<commit_message>
internal time for sikll
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Skill.xlsx
+++ b/_Out/NFDataCfg/Excel/Skill.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="458" windowWidth="27518" windowHeight="17543"/>
+    <workbookView xWindow="0" yWindow="458" windowWidth="27518" windowHeight="17543" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -30,15 +30,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Skill" type="4" refreshedVersion="2" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="Skill" type="4" refreshedVersion="2" background="1" saveData="1">
     <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\Skill.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="121">
   <si>
     <t>Id</t>
   </si>
@@ -402,11 +402,29 @@
     <t>缺省打击时间
 （本来应该打到但是物理没碰撞到或者其他原因）</t>
   </si>
+  <si>
+    <t>DamageCount</t>
+  </si>
+  <si>
+    <t>伤害count</t>
+  </si>
+  <si>
+    <t>DamageIntervalTime</t>
+  </si>
+  <si>
+    <t>only be used when damage count &gt; 1</t>
+  </si>
+  <si>
+    <t>0.6,0.6,0.6</t>
+  </si>
+  <si>
+    <t>0.6,0.6,0.7</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -599,7 +617,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -683,6 +701,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1029,13 +1050,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomLeft" activeCell="Y21" sqref="Y21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1047,23 +1068,23 @@
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" customWidth="1"/>
     <col min="8" max="8" width="17.73046875" customWidth="1"/>
-    <col min="9" max="11" width="20" customWidth="1"/>
-    <col min="12" max="12" width="17.1328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.19921875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.86328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.3984375" customWidth="1"/>
+    <col min="9" max="13" width="20" customWidth="1"/>
+    <col min="14" max="14" width="17.1328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.19921875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.86328125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.6640625" customWidth="1"/>
-    <col min="21" max="21" width="16.53125" customWidth="1"/>
-    <col min="22" max="22" width="22.9296875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.1328125" customWidth="1"/>
-    <col min="24" max="24" width="14.46484375" customWidth="1"/>
+    <col min="19" max="19" width="26.3984375" customWidth="1"/>
+    <col min="20" max="20" width="19" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.6640625" customWidth="1"/>
+    <col min="23" max="23" width="16.53125" customWidth="1"/>
+    <col min="24" max="24" width="22.9296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.1328125" customWidth="1"/>
+    <col min="26" max="26" width="14.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1">
+    <row r="1" spans="1:26" s="1" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1098,46 +1119,52 @@
         <v>10</v>
       </c>
       <c r="L1" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="2" customFormat="1">
+    <row r="2" spans="1:26" s="2" customFormat="1">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -1172,46 +1199,52 @@
         <v>23</v>
       </c>
       <c r="L2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="O2" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>25</v>
       </c>
       <c r="Q2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="T2" s="7" t="s">
         <v>24</v>
       </c>
       <c r="U2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="W2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="X2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="X2" s="7" t="s">
+      <c r="Y2" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" s="2" customFormat="1">
+      <c r="Z2" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" s="2" customFormat="1">
       <c r="A3" s="6" t="s">
         <v>26</v>
       </c>
@@ -1284,8 +1317,14 @@
       <c r="X3" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" s="2" customFormat="1">
+      <c r="Y3" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" s="2" customFormat="1">
       <c r="A4" s="6" t="s">
         <v>27</v>
       </c>
@@ -1358,8 +1397,14 @@
       <c r="X4" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" s="2" customFormat="1">
+      <c r="Y4" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" s="2" customFormat="1">
       <c r="A5" s="6" t="s">
         <v>28</v>
       </c>
@@ -1432,8 +1477,14 @@
       <c r="X5" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" s="2" customFormat="1">
+      <c r="Y5" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" s="2" customFormat="1">
       <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
@@ -1506,8 +1557,14 @@
       <c r="X6" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" s="3" customFormat="1">
+      <c r="Y6" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" s="3" customFormat="1">
       <c r="A7" s="8" t="s">
         <v>30</v>
       </c>
@@ -1580,8 +1637,14 @@
       <c r="X7" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" s="3" customFormat="1">
+      <c r="Y7" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" s="3" customFormat="1">
       <c r="A8" s="8" t="s">
         <v>109</v>
       </c>
@@ -1654,8 +1717,14 @@
       <c r="X8" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" s="3" customFormat="1">
+      <c r="Y8" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" s="3" customFormat="1">
       <c r="A9" s="8" t="s">
         <v>55</v>
       </c>
@@ -1728,8 +1797,14 @@
       <c r="X9" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" s="12" customFormat="1" ht="121.5">
+      <c r="Y9" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" s="12" customFormat="1" ht="121.5">
       <c r="A10" s="10" t="s">
         <v>4</v>
       </c>
@@ -1763,45 +1838,51 @@
       <c r="K10" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="L10" s="11" t="s">
+      <c r="L10" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="N10" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="M10" s="11" t="s">
+      <c r="O10" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="N10" s="11" t="s">
+      <c r="P10" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="O10" s="11" t="s">
+      <c r="Q10" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="P10" s="11" t="s">
+      <c r="R10" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="Q10" s="9" t="s">
+      <c r="S10" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="R10" s="11" t="s">
+      <c r="T10" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="S10" s="11" t="s">
+      <c r="U10" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="T10" s="11" t="s">
+      <c r="V10" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="U10" s="11" t="s">
+      <c r="W10" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="V10" s="11" t="s">
+      <c r="X10" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="W10" s="9" t="s">
+      <c r="Y10" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="X10" s="11"/>
-    </row>
-    <row r="11" spans="1:24" s="23" customFormat="1">
+      <c r="Z10" s="11"/>
+    </row>
+    <row r="11" spans="1:26" s="23" customFormat="1">
       <c r="A11" s="25" t="s">
         <v>98</v>
       </c>
@@ -1833,36 +1914,42 @@
       <c r="K11" s="22">
         <v>0</v>
       </c>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22">
-        <v>0</v>
-      </c>
-      <c r="O11" s="22">
-        <v>0</v>
-      </c>
+      <c r="L11" s="22">
+        <v>1</v>
+      </c>
+      <c r="M11" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
       <c r="P11" s="22">
         <v>0</v>
       </c>
       <c r="Q11" s="22">
         <v>0</v>
       </c>
-      <c r="R11" s="22"/>
-      <c r="S11" s="22"/>
-      <c r="T11" s="22" t="s">
+      <c r="R11" s="22">
+        <v>0</v>
+      </c>
+      <c r="S11" s="22">
+        <v>0</v>
+      </c>
+      <c r="T11" s="22"/>
+      <c r="U11" s="22"/>
+      <c r="V11" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="U11" s="22">
-        <v>0</v>
-      </c>
-      <c r="V11" s="22">
-        <v>1</v>
-      </c>
       <c r="W11" s="22">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" s="23" customFormat="1">
+        <v>0</v>
+      </c>
+      <c r="X11" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="22">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" s="23" customFormat="1">
       <c r="A12" s="25" t="s">
         <v>99</v>
       </c>
@@ -1894,36 +1981,42 @@
       <c r="K12" s="22">
         <v>0</v>
       </c>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22">
-        <v>0</v>
-      </c>
-      <c r="O12" s="22">
-        <v>0</v>
-      </c>
+      <c r="L12" s="22">
+        <v>1</v>
+      </c>
+      <c r="M12" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
       <c r="P12" s="22">
         <v>0</v>
       </c>
       <c r="Q12" s="22">
         <v>0</v>
       </c>
-      <c r="R12" s="22"/>
-      <c r="S12" s="22"/>
-      <c r="T12" s="22" t="s">
+      <c r="R12" s="22">
+        <v>0</v>
+      </c>
+      <c r="S12" s="22">
+        <v>0</v>
+      </c>
+      <c r="T12" s="22"/>
+      <c r="U12" s="22"/>
+      <c r="V12" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="U12" s="22">
-        <v>0</v>
-      </c>
-      <c r="V12" s="22">
-        <v>1</v>
-      </c>
       <c r="W12" s="22">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" s="23" customFormat="1">
+        <v>0</v>
+      </c>
+      <c r="X12" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="22">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" s="23" customFormat="1">
       <c r="A13" s="25" t="s">
         <v>100</v>
       </c>
@@ -1955,36 +2048,42 @@
       <c r="K13" s="22">
         <v>0</v>
       </c>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22">
-        <v>0</v>
-      </c>
-      <c r="O13" s="22">
-        <v>0</v>
-      </c>
+      <c r="L13" s="22">
+        <v>1</v>
+      </c>
+      <c r="M13" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="N13" s="22"/>
+      <c r="O13" s="22"/>
       <c r="P13" s="22">
         <v>0</v>
       </c>
       <c r="Q13" s="22">
         <v>0</v>
       </c>
-      <c r="R13" s="22"/>
-      <c r="S13" s="22"/>
-      <c r="T13" s="22" t="s">
+      <c r="R13" s="22">
+        <v>0</v>
+      </c>
+      <c r="S13" s="22">
+        <v>0</v>
+      </c>
+      <c r="T13" s="22"/>
+      <c r="U13" s="22"/>
+      <c r="V13" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="U13" s="22">
-        <v>0</v>
-      </c>
-      <c r="V13" s="22">
-        <v>1</v>
-      </c>
       <c r="W13" s="22">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" s="23" customFormat="1">
+        <v>0</v>
+      </c>
+      <c r="X13" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="22">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" s="23" customFormat="1">
       <c r="A14" s="25" t="s">
         <v>101</v>
       </c>
@@ -2016,36 +2115,42 @@
       <c r="K14" s="22">
         <v>0</v>
       </c>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22">
-        <v>0</v>
-      </c>
-      <c r="O14" s="22">
-        <v>0</v>
-      </c>
+      <c r="L14" s="22">
+        <v>1</v>
+      </c>
+      <c r="M14" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
       <c r="P14" s="22">
         <v>0</v>
       </c>
       <c r="Q14" s="22">
         <v>0</v>
       </c>
-      <c r="R14" s="22"/>
-      <c r="S14" s="22"/>
-      <c r="T14" s="22" t="s">
+      <c r="R14" s="22">
+        <v>0</v>
+      </c>
+      <c r="S14" s="22">
+        <v>0</v>
+      </c>
+      <c r="T14" s="22"/>
+      <c r="U14" s="22"/>
+      <c r="V14" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="U14" s="22">
-        <v>0</v>
-      </c>
-      <c r="V14" s="22">
-        <v>1</v>
-      </c>
       <c r="W14" s="22">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" s="23" customFormat="1">
+        <v>0</v>
+      </c>
+      <c r="X14" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="22">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" s="23" customFormat="1">
       <c r="A15" s="25" t="s">
         <v>102</v>
       </c>
@@ -2077,36 +2182,42 @@
       <c r="K15" s="22">
         <v>0</v>
       </c>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22">
-        <v>0</v>
-      </c>
-      <c r="O15" s="22">
-        <v>0</v>
-      </c>
+      <c r="L15" s="22">
+        <v>1</v>
+      </c>
+      <c r="M15" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
       <c r="P15" s="22">
         <v>0</v>
       </c>
       <c r="Q15" s="22">
         <v>0</v>
       </c>
-      <c r="R15" s="22"/>
-      <c r="S15" s="22"/>
-      <c r="T15" s="22" t="s">
+      <c r="R15" s="22">
+        <v>0</v>
+      </c>
+      <c r="S15" s="22">
+        <v>0</v>
+      </c>
+      <c r="T15" s="22"/>
+      <c r="U15" s="22"/>
+      <c r="V15" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="U15" s="22">
-        <v>0</v>
-      </c>
-      <c r="V15" s="22">
-        <v>1</v>
-      </c>
       <c r="W15" s="22">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" s="23" customFormat="1">
+        <v>0</v>
+      </c>
+      <c r="X15" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y15" s="22">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" s="23" customFormat="1">
       <c r="A16" s="25" t="s">
         <v>103</v>
       </c>
@@ -2138,36 +2249,42 @@
       <c r="K16" s="22">
         <v>0</v>
       </c>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22">
-        <v>0</v>
-      </c>
-      <c r="O16" s="22">
-        <v>0</v>
-      </c>
+      <c r="L16" s="22">
+        <v>1</v>
+      </c>
+      <c r="M16" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
       <c r="P16" s="22">
         <v>0</v>
       </c>
       <c r="Q16" s="22">
         <v>0</v>
       </c>
-      <c r="R16" s="22"/>
-      <c r="S16" s="22"/>
-      <c r="T16" s="22" t="s">
+      <c r="R16" s="22">
+        <v>0</v>
+      </c>
+      <c r="S16" s="22">
+        <v>0</v>
+      </c>
+      <c r="T16" s="22"/>
+      <c r="U16" s="22"/>
+      <c r="V16" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="U16" s="22">
-        <v>0</v>
-      </c>
-      <c r="V16" s="22">
-        <v>1</v>
-      </c>
       <c r="W16" s="22">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" s="23" customFormat="1">
+        <v>0</v>
+      </c>
+      <c r="X16" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y16" s="22">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" s="23" customFormat="1">
       <c r="A17" s="25" t="s">
         <v>104</v>
       </c>
@@ -2199,36 +2316,42 @@
       <c r="K17" s="22">
         <v>0</v>
       </c>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22">
-        <v>0</v>
-      </c>
-      <c r="O17" s="22">
-        <v>0</v>
-      </c>
+      <c r="L17" s="22">
+        <v>1</v>
+      </c>
+      <c r="M17" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
       <c r="P17" s="22">
         <v>0</v>
       </c>
       <c r="Q17" s="22">
         <v>0</v>
       </c>
-      <c r="R17" s="22"/>
-      <c r="S17" s="22"/>
-      <c r="T17" s="22" t="s">
+      <c r="R17" s="22">
+        <v>0</v>
+      </c>
+      <c r="S17" s="22">
+        <v>0</v>
+      </c>
+      <c r="T17" s="22"/>
+      <c r="U17" s="22"/>
+      <c r="V17" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="U17" s="22">
-        <v>0</v>
-      </c>
-      <c r="V17" s="22">
-        <v>1</v>
-      </c>
       <c r="W17" s="22">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" s="23" customFormat="1">
+        <v>0</v>
+      </c>
+      <c r="X17" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="22">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" s="23" customFormat="1">
       <c r="A18" s="25" t="s">
         <v>105</v>
       </c>
@@ -2260,36 +2383,42 @@
       <c r="K18" s="22">
         <v>0</v>
       </c>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22">
-        <v>0</v>
-      </c>
-      <c r="O18" s="22">
-        <v>0</v>
-      </c>
+      <c r="L18" s="22">
+        <v>1</v>
+      </c>
+      <c r="M18" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
       <c r="P18" s="22">
         <v>0</v>
       </c>
       <c r="Q18" s="22">
         <v>0</v>
       </c>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
-      <c r="T18" s="22" t="s">
+      <c r="R18" s="22">
+        <v>0</v>
+      </c>
+      <c r="S18" s="22">
+        <v>0</v>
+      </c>
+      <c r="T18" s="22"/>
+      <c r="U18" s="22"/>
+      <c r="V18" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="U18" s="22">
-        <v>0</v>
-      </c>
-      <c r="V18" s="22">
-        <v>1</v>
-      </c>
       <c r="W18" s="22">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" s="23" customFormat="1">
+        <v>0</v>
+      </c>
+      <c r="X18" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="22">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" s="23" customFormat="1">
       <c r="A19" s="25" t="s">
         <v>106</v>
       </c>
@@ -2321,36 +2450,42 @@
       <c r="K19" s="22">
         <v>0</v>
       </c>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22">
-        <v>1</v>
-      </c>
-      <c r="O19" s="22">
-        <v>0</v>
-      </c>
+      <c r="L19" s="22">
+        <v>1</v>
+      </c>
+      <c r="M19" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="N19" s="22"/>
+      <c r="O19" s="22"/>
       <c r="P19" s="22">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="22">
+        <v>0</v>
+      </c>
+      <c r="R19" s="22">
         <v>2</v>
       </c>
-      <c r="Q19" s="22">
-        <v>0</v>
-      </c>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
-      <c r="T19" s="22" t="s">
+      <c r="S19" s="22">
+        <v>0</v>
+      </c>
+      <c r="T19" s="22"/>
+      <c r="U19" s="22"/>
+      <c r="V19" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="U19" s="22">
-        <v>0</v>
-      </c>
-      <c r="V19" s="22">
-        <v>1</v>
-      </c>
       <c r="W19" s="22">
+        <v>0</v>
+      </c>
+      <c r="X19" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="22">
         <v>0.6</v>
       </c>
     </row>
-    <row r="20" spans="1:23" s="14" customFormat="1">
+    <row r="20" spans="1:25" s="14" customFormat="1">
       <c r="A20" s="13" t="s">
         <v>56</v>
       </c>
@@ -2382,36 +2517,42 @@
       <c r="K20" s="13">
         <v>0</v>
       </c>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13">
-        <v>0</v>
-      </c>
-      <c r="O20" s="13">
-        <v>0</v>
-      </c>
+      <c r="L20" s="13">
+        <v>1</v>
+      </c>
+      <c r="M20" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
       <c r="P20" s="13">
         <v>0</v>
       </c>
       <c r="Q20" s="13">
         <v>0</v>
       </c>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13"/>
-      <c r="T20" s="13" t="s">
+      <c r="R20" s="13">
+        <v>0</v>
+      </c>
+      <c r="S20" s="13">
+        <v>0</v>
+      </c>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U20" s="13">
-        <v>0</v>
-      </c>
-      <c r="V20" s="13">
-        <v>1</v>
-      </c>
       <c r="W20" s="13">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" s="14" customFormat="1">
+        <v>0</v>
+      </c>
+      <c r="X20" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" s="14" customFormat="1">
       <c r="A21" s="13" t="s">
         <v>57</v>
       </c>
@@ -2443,36 +2584,42 @@
       <c r="K21" s="13">
         <v>0</v>
       </c>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13">
-        <v>0</v>
-      </c>
-      <c r="O21" s="13">
-        <v>0</v>
-      </c>
+      <c r="L21" s="13">
+        <v>1</v>
+      </c>
+      <c r="M21" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
       <c r="P21" s="13">
         <v>0</v>
       </c>
       <c r="Q21" s="13">
         <v>0</v>
       </c>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13" t="s">
+      <c r="R21" s="13">
+        <v>0</v>
+      </c>
+      <c r="S21" s="13">
+        <v>0</v>
+      </c>
+      <c r="T21" s="13"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U21" s="13">
-        <v>0</v>
-      </c>
-      <c r="V21" s="13">
-        <v>1</v>
-      </c>
       <c r="W21" s="13">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" s="14" customFormat="1">
+        <v>0</v>
+      </c>
+      <c r="X21" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" s="14" customFormat="1">
       <c r="A22" s="13" t="s">
         <v>58</v>
       </c>
@@ -2504,36 +2651,42 @@
       <c r="K22" s="13">
         <v>0</v>
       </c>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13">
-        <v>0</v>
-      </c>
-      <c r="O22" s="13">
-        <v>0</v>
-      </c>
+      <c r="L22" s="13">
+        <v>1</v>
+      </c>
+      <c r="M22" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
       <c r="P22" s="13">
         <v>0</v>
       </c>
       <c r="Q22" s="13">
         <v>0</v>
       </c>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13" t="s">
+      <c r="R22" s="13">
+        <v>0</v>
+      </c>
+      <c r="S22" s="13">
+        <v>0</v>
+      </c>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U22" s="13">
-        <v>0</v>
-      </c>
-      <c r="V22" s="13">
-        <v>1</v>
-      </c>
       <c r="W22" s="13">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" s="14" customFormat="1">
+        <v>0</v>
+      </c>
+      <c r="X22" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y22" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" s="14" customFormat="1">
       <c r="A23" s="13" t="s">
         <v>59</v>
       </c>
@@ -2565,36 +2718,42 @@
       <c r="K23" s="13">
         <v>0</v>
       </c>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13">
-        <v>0</v>
-      </c>
-      <c r="O23" s="13">
-        <v>0</v>
-      </c>
+      <c r="L23" s="13">
+        <v>1</v>
+      </c>
+      <c r="M23" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
       <c r="P23" s="13">
         <v>0</v>
       </c>
       <c r="Q23" s="13">
         <v>0</v>
       </c>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
-      <c r="T23" s="13" t="s">
+      <c r="R23" s="13">
+        <v>0</v>
+      </c>
+      <c r="S23" s="13">
+        <v>0</v>
+      </c>
+      <c r="T23" s="13"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U23" s="13">
-        <v>0</v>
-      </c>
-      <c r="V23" s="13">
-        <v>1</v>
-      </c>
       <c r="W23" s="13">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" s="14" customFormat="1">
+        <v>0</v>
+      </c>
+      <c r="X23" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" s="14" customFormat="1">
       <c r="A24" s="13" t="s">
         <v>60</v>
       </c>
@@ -2626,36 +2785,42 @@
       <c r="K24" s="13">
         <v>0</v>
       </c>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13">
-        <v>0</v>
-      </c>
-      <c r="O24" s="13">
-        <v>0</v>
-      </c>
+      <c r="L24" s="13">
+        <v>1</v>
+      </c>
+      <c r="M24" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
       <c r="P24" s="13">
         <v>0</v>
       </c>
       <c r="Q24" s="13">
         <v>0</v>
       </c>
-      <c r="R24" s="13"/>
-      <c r="S24" s="13"/>
-      <c r="T24" s="13" t="s">
+      <c r="R24" s="13">
+        <v>0</v>
+      </c>
+      <c r="S24" s="13">
+        <v>0</v>
+      </c>
+      <c r="T24" s="13"/>
+      <c r="U24" s="13"/>
+      <c r="V24" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U24" s="13">
-        <v>0</v>
-      </c>
-      <c r="V24" s="13">
-        <v>1</v>
-      </c>
       <c r="W24" s="13">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" s="14" customFormat="1">
+        <v>0</v>
+      </c>
+      <c r="X24" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" s="14" customFormat="1">
       <c r="A25" s="13" t="s">
         <v>61</v>
       </c>
@@ -2687,36 +2852,42 @@
       <c r="K25" s="13">
         <v>0</v>
       </c>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13">
-        <v>0</v>
-      </c>
-      <c r="O25" s="13">
-        <v>0</v>
-      </c>
+      <c r="L25" s="13">
+        <v>1</v>
+      </c>
+      <c r="M25" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
       <c r="P25" s="13">
         <v>0</v>
       </c>
       <c r="Q25" s="13">
         <v>0</v>
       </c>
-      <c r="R25" s="13"/>
-      <c r="S25" s="13"/>
-      <c r="T25" s="13" t="s">
+      <c r="R25" s="13">
+        <v>0</v>
+      </c>
+      <c r="S25" s="13">
+        <v>0</v>
+      </c>
+      <c r="T25" s="13"/>
+      <c r="U25" s="13"/>
+      <c r="V25" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U25" s="13">
-        <v>0</v>
-      </c>
-      <c r="V25" s="13">
-        <v>1</v>
-      </c>
       <c r="W25" s="13">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" s="14" customFormat="1">
+        <v>0</v>
+      </c>
+      <c r="X25" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" s="14" customFormat="1">
       <c r="A26" s="13" t="s">
         <v>62</v>
       </c>
@@ -2748,36 +2919,42 @@
       <c r="K26" s="13">
         <v>0</v>
       </c>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13">
-        <v>0</v>
-      </c>
-      <c r="O26" s="13">
-        <v>0</v>
-      </c>
+      <c r="L26" s="13">
+        <v>1</v>
+      </c>
+      <c r="M26" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
       <c r="P26" s="13">
         <v>0</v>
       </c>
       <c r="Q26" s="13">
         <v>0</v>
       </c>
-      <c r="R26" s="13"/>
-      <c r="S26" s="13"/>
-      <c r="T26" s="13" t="s">
+      <c r="R26" s="13">
+        <v>0</v>
+      </c>
+      <c r="S26" s="13">
+        <v>0</v>
+      </c>
+      <c r="T26" s="13"/>
+      <c r="U26" s="13"/>
+      <c r="V26" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U26" s="13">
-        <v>0</v>
-      </c>
-      <c r="V26" s="13">
-        <v>1</v>
-      </c>
       <c r="W26" s="13">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" s="14" customFormat="1">
+        <v>0</v>
+      </c>
+      <c r="X26" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" s="14" customFormat="1">
       <c r="A27" s="13" t="s">
         <v>63</v>
       </c>
@@ -2809,36 +2986,42 @@
       <c r="K27" s="13">
         <v>0</v>
       </c>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13">
-        <v>0</v>
-      </c>
-      <c r="O27" s="13">
-        <v>0</v>
-      </c>
+      <c r="L27" s="13">
+        <v>1</v>
+      </c>
+      <c r="M27" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
       <c r="P27" s="13">
         <v>0</v>
       </c>
       <c r="Q27" s="13">
         <v>0</v>
       </c>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13" t="s">
+      <c r="R27" s="13">
+        <v>0</v>
+      </c>
+      <c r="S27" s="13">
+        <v>0</v>
+      </c>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U27" s="13">
-        <v>0</v>
-      </c>
-      <c r="V27" s="13">
-        <v>1</v>
-      </c>
       <c r="W27" s="13">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" s="14" customFormat="1">
+        <v>0</v>
+      </c>
+      <c r="X27" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" s="14" customFormat="1">
       <c r="A28" s="13" t="s">
         <v>64</v>
       </c>
@@ -2870,36 +3053,42 @@
       <c r="K28" s="13">
         <v>0</v>
       </c>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13">
-        <v>1</v>
-      </c>
-      <c r="O28" s="13">
-        <v>0</v>
-      </c>
+      <c r="L28" s="13">
+        <v>1</v>
+      </c>
+      <c r="M28" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
       <c r="P28" s="13">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="13">
+        <v>0</v>
+      </c>
+      <c r="R28" s="13">
         <v>2</v>
       </c>
-      <c r="Q28" s="13">
-        <v>0</v>
-      </c>
-      <c r="R28" s="13"/>
-      <c r="S28" s="13"/>
-      <c r="T28" s="13" t="s">
+      <c r="S28" s="13">
+        <v>0</v>
+      </c>
+      <c r="T28" s="13"/>
+      <c r="U28" s="13"/>
+      <c r="V28" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U28" s="13">
-        <v>0</v>
-      </c>
-      <c r="V28" s="13">
-        <v>1</v>
-      </c>
       <c r="W28" s="13">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" s="17" customFormat="1">
+        <v>0</v>
+      </c>
+      <c r="X28" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y28" s="28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" s="17" customFormat="1">
       <c r="A29" s="16" t="s">
         <v>65</v>
       </c>
@@ -2927,35 +3116,41 @@
       <c r="K29" s="18">
         <v>0</v>
       </c>
-      <c r="N29" s="18">
-        <v>1</v>
-      </c>
-      <c r="O29" s="17">
-        <v>0</v>
+      <c r="L29" s="18">
+        <v>1</v>
+      </c>
+      <c r="M29" s="18">
+        <v>0.3</v>
       </c>
       <c r="P29" s="18">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="17">
+        <v>0</v>
+      </c>
+      <c r="R29" s="18">
         <v>2</v>
       </c>
-      <c r="Q29" s="18">
-        <v>0</v>
-      </c>
-      <c r="S29" s="17" t="s">
+      <c r="S29" s="18">
+        <v>0</v>
+      </c>
+      <c r="U29" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="T29" s="13" t="s">
+      <c r="V29" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U29" s="17">
-        <v>0</v>
-      </c>
-      <c r="V29" s="17">
-        <v>1</v>
-      </c>
-      <c r="W29" s="18">
+      <c r="W29" s="17">
+        <v>0</v>
+      </c>
+      <c r="X29" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y29" s="18">
         <v>0.6</v>
       </c>
     </row>
-    <row r="30" spans="1:23" s="17" customFormat="1">
+    <row r="30" spans="1:25" s="17" customFormat="1">
       <c r="A30" s="16" t="s">
         <v>66</v>
       </c>
@@ -2983,35 +3178,41 @@
       <c r="K30" s="18">
         <v>0</v>
       </c>
-      <c r="N30" s="18">
-        <v>1</v>
-      </c>
-      <c r="O30" s="17">
-        <v>0</v>
+      <c r="L30" s="18">
+        <v>1</v>
+      </c>
+      <c r="M30" s="18">
+        <v>0.3</v>
       </c>
       <c r="P30" s="18">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="17">
+        <v>0</v>
+      </c>
+      <c r="R30" s="18">
         <v>2</v>
       </c>
-      <c r="Q30" s="18">
-        <v>0</v>
-      </c>
-      <c r="S30" s="17" t="s">
+      <c r="S30" s="18">
+        <v>0</v>
+      </c>
+      <c r="U30" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="T30" s="13" t="s">
+      <c r="V30" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U30" s="17">
-        <v>0</v>
-      </c>
-      <c r="V30" s="17">
-        <v>1</v>
-      </c>
-      <c r="W30" s="18">
+      <c r="W30" s="17">
+        <v>0</v>
+      </c>
+      <c r="X30" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y30" s="18">
         <v>0.6</v>
       </c>
     </row>
-    <row r="31" spans="1:23" s="17" customFormat="1">
+    <row r="31" spans="1:25" s="17" customFormat="1">
       <c r="A31" s="16" t="s">
         <v>67</v>
       </c>
@@ -3039,35 +3240,41 @@
       <c r="K31" s="18">
         <v>0</v>
       </c>
-      <c r="N31" s="18">
-        <v>1</v>
-      </c>
-      <c r="O31" s="17">
-        <v>0</v>
+      <c r="L31" s="18">
+        <v>1</v>
+      </c>
+      <c r="M31" s="18">
+        <v>0.3</v>
       </c>
       <c r="P31" s="18">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="17">
+        <v>0</v>
+      </c>
+      <c r="R31" s="18">
         <v>2</v>
       </c>
-      <c r="Q31" s="18">
-        <v>0</v>
-      </c>
-      <c r="S31" s="17" t="s">
+      <c r="S31" s="18">
+        <v>0</v>
+      </c>
+      <c r="U31" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="T31" s="13" t="s">
+      <c r="V31" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U31" s="17">
-        <v>0</v>
-      </c>
-      <c r="V31" s="17">
-        <v>1</v>
-      </c>
-      <c r="W31" s="18">
+      <c r="W31" s="17">
+        <v>0</v>
+      </c>
+      <c r="X31" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y31" s="18">
         <v>0.6</v>
       </c>
     </row>
-    <row r="32" spans="1:23" s="17" customFormat="1">
+    <row r="32" spans="1:25" s="17" customFormat="1">
       <c r="A32" s="16" t="s">
         <v>68</v>
       </c>
@@ -3095,32 +3302,38 @@
       <c r="K32" s="18">
         <v>0</v>
       </c>
-      <c r="N32" s="18">
-        <v>1</v>
-      </c>
-      <c r="O32" s="17">
-        <v>0</v>
+      <c r="L32" s="18">
+        <v>1</v>
+      </c>
+      <c r="M32" s="18">
+        <v>0.3</v>
       </c>
       <c r="P32" s="18">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="17">
+        <v>0</v>
+      </c>
+      <c r="R32" s="18">
         <v>2</v>
       </c>
-      <c r="Q32" s="18">
-        <v>0</v>
-      </c>
-      <c r="T32" s="13" t="s">
+      <c r="S32" s="18">
+        <v>0</v>
+      </c>
+      <c r="V32" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U32" s="17">
-        <v>0</v>
-      </c>
-      <c r="V32" s="17">
-        <v>1</v>
-      </c>
-      <c r="W32" s="18">
+      <c r="W32" s="17">
+        <v>0</v>
+      </c>
+      <c r="X32" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y32" s="18">
         <v>0.6</v>
       </c>
     </row>
-    <row r="33" spans="1:23" s="17" customFormat="1">
+    <row r="33" spans="1:25" s="17" customFormat="1">
       <c r="A33" s="16" t="s">
         <v>69</v>
       </c>
@@ -3148,32 +3361,38 @@
       <c r="K33" s="18">
         <v>0</v>
       </c>
-      <c r="N33" s="18">
-        <v>1</v>
-      </c>
-      <c r="O33" s="17">
-        <v>0</v>
+      <c r="L33" s="18">
+        <v>1</v>
+      </c>
+      <c r="M33" s="18">
+        <v>0.3</v>
       </c>
       <c r="P33" s="18">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="17">
+        <v>0</v>
+      </c>
+      <c r="R33" s="18">
         <v>2</v>
       </c>
-      <c r="Q33" s="18">
-        <v>0</v>
-      </c>
-      <c r="T33" s="13" t="s">
+      <c r="S33" s="18">
+        <v>0</v>
+      </c>
+      <c r="V33" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U33" s="17">
-        <v>0</v>
-      </c>
-      <c r="V33" s="17">
-        <v>1</v>
-      </c>
-      <c r="W33" s="18">
+      <c r="W33" s="17">
+        <v>0</v>
+      </c>
+      <c r="X33" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y33" s="18">
         <v>0.6</v>
       </c>
     </row>
-    <row r="34" spans="1:23" s="17" customFormat="1">
+    <row r="34" spans="1:25" s="17" customFormat="1">
       <c r="A34" s="16" t="s">
         <v>70</v>
       </c>
@@ -3201,32 +3420,38 @@
       <c r="K34" s="18">
         <v>0</v>
       </c>
-      <c r="N34" s="18">
-        <v>1</v>
-      </c>
-      <c r="O34" s="17">
-        <v>0</v>
+      <c r="L34" s="18">
+        <v>1</v>
+      </c>
+      <c r="M34" s="18">
+        <v>0.3</v>
       </c>
       <c r="P34" s="18">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="17">
+        <v>0</v>
+      </c>
+      <c r="R34" s="18">
         <v>2</v>
       </c>
-      <c r="Q34" s="18">
-        <v>0</v>
-      </c>
-      <c r="T34" s="13" t="s">
+      <c r="S34" s="18">
+        <v>0</v>
+      </c>
+      <c r="V34" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U34" s="17">
-        <v>0</v>
-      </c>
-      <c r="V34" s="17">
-        <v>1</v>
-      </c>
-      <c r="W34" s="18">
+      <c r="W34" s="17">
+        <v>0</v>
+      </c>
+      <c r="X34" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y34" s="18">
         <v>0.6</v>
       </c>
     </row>
-    <row r="35" spans="1:23" s="17" customFormat="1">
+    <row r="35" spans="1:25" s="17" customFormat="1">
       <c r="A35" s="16" t="s">
         <v>71</v>
       </c>
@@ -3254,32 +3479,38 @@
       <c r="K35" s="18">
         <v>0</v>
       </c>
-      <c r="N35" s="18">
-        <v>1</v>
-      </c>
-      <c r="O35" s="17">
-        <v>0</v>
+      <c r="L35" s="18">
+        <v>1</v>
+      </c>
+      <c r="M35" s="18">
+        <v>0.3</v>
       </c>
       <c r="P35" s="18">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="17">
+        <v>0</v>
+      </c>
+      <c r="R35" s="18">
         <v>2</v>
       </c>
-      <c r="Q35" s="18">
-        <v>0</v>
-      </c>
-      <c r="T35" s="13" t="s">
+      <c r="S35" s="18">
+        <v>0</v>
+      </c>
+      <c r="V35" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U35" s="17">
-        <v>0</v>
-      </c>
-      <c r="V35" s="17">
-        <v>1</v>
-      </c>
-      <c r="W35" s="18">
+      <c r="W35" s="17">
+        <v>0</v>
+      </c>
+      <c r="X35" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y35" s="18">
         <v>0.6</v>
       </c>
     </row>
-    <row r="36" spans="1:23" s="17" customFormat="1">
+    <row r="36" spans="1:25" s="17" customFormat="1">
       <c r="A36" s="16" t="s">
         <v>72</v>
       </c>
@@ -3307,32 +3538,38 @@
       <c r="K36" s="18">
         <v>0</v>
       </c>
-      <c r="N36" s="18">
-        <v>1</v>
-      </c>
-      <c r="O36" s="17">
-        <v>0</v>
+      <c r="L36" s="18">
+        <v>1</v>
+      </c>
+      <c r="M36" s="18">
+        <v>0.3</v>
       </c>
       <c r="P36" s="18">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="17">
+        <v>0</v>
+      </c>
+      <c r="R36" s="18">
         <v>2</v>
       </c>
-      <c r="Q36" s="18">
-        <v>0</v>
-      </c>
-      <c r="T36" s="13" t="s">
+      <c r="S36" s="18">
+        <v>0</v>
+      </c>
+      <c r="V36" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U36" s="17">
-        <v>0</v>
-      </c>
-      <c r="V36" s="17">
-        <v>1</v>
-      </c>
-      <c r="W36" s="18">
+      <c r="W36" s="17">
+        <v>0</v>
+      </c>
+      <c r="X36" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y36" s="18">
         <v>0.6</v>
       </c>
     </row>
-    <row r="37" spans="1:23" s="17" customFormat="1">
+    <row r="37" spans="1:25" s="17" customFormat="1">
       <c r="A37" s="16" t="s">
         <v>73</v>
       </c>
@@ -3360,32 +3597,38 @@
       <c r="K37" s="18">
         <v>0</v>
       </c>
-      <c r="N37" s="18">
-        <v>1</v>
-      </c>
-      <c r="O37" s="17">
-        <v>0</v>
+      <c r="L37" s="18">
+        <v>1</v>
+      </c>
+      <c r="M37" s="18">
+        <v>0.3</v>
       </c>
       <c r="P37" s="18">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="17">
+        <v>0</v>
+      </c>
+      <c r="R37" s="18">
         <v>2</v>
       </c>
-      <c r="Q37" s="18">
-        <v>0</v>
-      </c>
-      <c r="T37" s="13" t="s">
+      <c r="S37" s="18">
+        <v>0</v>
+      </c>
+      <c r="V37" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U37" s="17">
-        <v>0</v>
-      </c>
-      <c r="V37" s="17">
-        <v>1</v>
-      </c>
-      <c r="W37" s="18">
+      <c r="W37" s="17">
+        <v>0</v>
+      </c>
+      <c r="X37" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y37" s="18">
         <v>0.6</v>
       </c>
     </row>
-    <row r="38" spans="1:23" s="20" customFormat="1" ht="17.649999999999999">
+    <row r="38" spans="1:25" s="20" customFormat="1" ht="17.649999999999999">
       <c r="A38" s="19" t="s">
         <v>74</v>
       </c>
@@ -3414,35 +3657,41 @@
       <c r="K38" s="21">
         <v>0</v>
       </c>
-      <c r="N38" s="21">
-        <v>1</v>
-      </c>
-      <c r="O38" s="20">
-        <v>0</v>
+      <c r="L38" s="21">
+        <v>1</v>
+      </c>
+      <c r="M38" s="21">
+        <v>0.3</v>
       </c>
       <c r="P38" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="20">
+        <v>0</v>
+      </c>
+      <c r="R38" s="21">
         <v>2</v>
       </c>
-      <c r="Q38" s="21">
-        <v>0</v>
-      </c>
-      <c r="S38" s="20" t="s">
+      <c r="S38" s="21">
+        <v>0</v>
+      </c>
+      <c r="U38" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="T38" s="13" t="s">
+      <c r="V38" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U38" s="20">
-        <v>0</v>
-      </c>
-      <c r="V38" s="20">
-        <v>1</v>
-      </c>
-      <c r="W38" s="21">
+      <c r="W38" s="20">
+        <v>0</v>
+      </c>
+      <c r="X38" s="20">
+        <v>1</v>
+      </c>
+      <c r="Y38" s="21">
         <v>0.6</v>
       </c>
     </row>
-    <row r="39" spans="1:23" s="20" customFormat="1" ht="17.649999999999999">
+    <row r="39" spans="1:25" s="20" customFormat="1" ht="17.649999999999999">
       <c r="A39" s="19" t="s">
         <v>75</v>
       </c>
@@ -3471,35 +3720,41 @@
       <c r="K39" s="21">
         <v>0</v>
       </c>
-      <c r="N39" s="21">
-        <v>1</v>
-      </c>
-      <c r="O39" s="20">
-        <v>0</v>
+      <c r="L39" s="21">
+        <v>1</v>
+      </c>
+      <c r="M39" s="21">
+        <v>0.3</v>
       </c>
       <c r="P39" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="20">
+        <v>0</v>
+      </c>
+      <c r="R39" s="21">
         <v>2</v>
       </c>
-      <c r="Q39" s="21">
-        <v>0</v>
-      </c>
-      <c r="S39" s="20" t="s">
+      <c r="S39" s="21">
+        <v>0</v>
+      </c>
+      <c r="U39" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="T39" s="13" t="s">
+      <c r="V39" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U39" s="20">
-        <v>0</v>
-      </c>
-      <c r="V39" s="20">
-        <v>1</v>
-      </c>
-      <c r="W39" s="21">
+      <c r="W39" s="20">
+        <v>0</v>
+      </c>
+      <c r="X39" s="20">
+        <v>1</v>
+      </c>
+      <c r="Y39" s="21">
         <v>0.6</v>
       </c>
     </row>
-    <row r="40" spans="1:23" s="20" customFormat="1" ht="17.649999999999999">
+    <row r="40" spans="1:25" s="20" customFormat="1" ht="17.649999999999999">
       <c r="A40" s="19" t="s">
         <v>76</v>
       </c>
@@ -3528,35 +3783,41 @@
       <c r="K40" s="21">
         <v>0</v>
       </c>
-      <c r="N40" s="21">
-        <v>1</v>
-      </c>
-      <c r="O40" s="20">
-        <v>0</v>
+      <c r="L40" s="21">
+        <v>1</v>
+      </c>
+      <c r="M40" s="21">
+        <v>0.3</v>
       </c>
       <c r="P40" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="20">
+        <v>0</v>
+      </c>
+      <c r="R40" s="21">
         <v>2</v>
       </c>
-      <c r="Q40" s="21">
-        <v>0</v>
-      </c>
-      <c r="S40" s="20" t="s">
+      <c r="S40" s="21">
+        <v>0</v>
+      </c>
+      <c r="U40" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="T40" s="13" t="s">
+      <c r="V40" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U40" s="20">
-        <v>0</v>
-      </c>
-      <c r="V40" s="20">
-        <v>1</v>
-      </c>
-      <c r="W40" s="21">
+      <c r="W40" s="20">
+        <v>0</v>
+      </c>
+      <c r="X40" s="20">
+        <v>1</v>
+      </c>
+      <c r="Y40" s="21">
         <v>0.6</v>
       </c>
     </row>
-    <row r="41" spans="1:23" s="20" customFormat="1" ht="17.649999999999999">
+    <row r="41" spans="1:25" s="20" customFormat="1" ht="17.649999999999999">
       <c r="A41" s="19" t="s">
         <v>77</v>
       </c>
@@ -3585,32 +3846,38 @@
       <c r="K41" s="21">
         <v>0</v>
       </c>
-      <c r="N41" s="21">
-        <v>1</v>
-      </c>
-      <c r="O41" s="20">
-        <v>0</v>
+      <c r="L41" s="21">
+        <v>1</v>
+      </c>
+      <c r="M41" s="21">
+        <v>0.3</v>
       </c>
       <c r="P41" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="20">
+        <v>0</v>
+      </c>
+      <c r="R41" s="21">
         <v>2</v>
       </c>
-      <c r="Q41" s="21">
-        <v>0</v>
-      </c>
-      <c r="T41" s="13" t="s">
+      <c r="S41" s="21">
+        <v>0</v>
+      </c>
+      <c r="V41" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U41" s="20">
-        <v>0</v>
-      </c>
-      <c r="V41" s="20">
-        <v>1</v>
-      </c>
-      <c r="W41" s="21">
+      <c r="W41" s="20">
+        <v>0</v>
+      </c>
+      <c r="X41" s="20">
+        <v>1</v>
+      </c>
+      <c r="Y41" s="21">
         <v>0.6</v>
       </c>
     </row>
-    <row r="42" spans="1:23" s="20" customFormat="1" ht="17.649999999999999">
+    <row r="42" spans="1:25" s="20" customFormat="1" ht="17.649999999999999">
       <c r="A42" s="19" t="s">
         <v>78</v>
       </c>
@@ -3639,32 +3906,38 @@
       <c r="K42" s="21">
         <v>0</v>
       </c>
-      <c r="N42" s="21">
-        <v>1</v>
-      </c>
-      <c r="O42" s="20">
-        <v>0</v>
+      <c r="L42" s="21">
+        <v>1</v>
+      </c>
+      <c r="M42" s="21">
+        <v>0.3</v>
       </c>
       <c r="P42" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="20">
+        <v>0</v>
+      </c>
+      <c r="R42" s="21">
         <v>2</v>
       </c>
-      <c r="Q42" s="21">
-        <v>0</v>
-      </c>
-      <c r="T42" s="13" t="s">
+      <c r="S42" s="21">
+        <v>0</v>
+      </c>
+      <c r="V42" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U42" s="20">
-        <v>0</v>
-      </c>
-      <c r="V42" s="20">
-        <v>1</v>
-      </c>
-      <c r="W42" s="21">
+      <c r="W42" s="20">
+        <v>0</v>
+      </c>
+      <c r="X42" s="20">
+        <v>1</v>
+      </c>
+      <c r="Y42" s="21">
         <v>0.6</v>
       </c>
     </row>
-    <row r="43" spans="1:23" s="20" customFormat="1" ht="17.649999999999999">
+    <row r="43" spans="1:25" s="20" customFormat="1" ht="17.649999999999999">
       <c r="A43" s="19" t="s">
         <v>79</v>
       </c>
@@ -3693,32 +3966,38 @@
       <c r="K43" s="21">
         <v>0</v>
       </c>
-      <c r="N43" s="21">
-        <v>1</v>
-      </c>
-      <c r="O43" s="20">
-        <v>0</v>
+      <c r="L43" s="21">
+        <v>1</v>
+      </c>
+      <c r="M43" s="21">
+        <v>0.3</v>
       </c>
       <c r="P43" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q43" s="20">
+        <v>0</v>
+      </c>
+      <c r="R43" s="21">
         <v>2</v>
       </c>
-      <c r="Q43" s="21">
-        <v>0</v>
-      </c>
-      <c r="T43" s="13" t="s">
+      <c r="S43" s="21">
+        <v>0</v>
+      </c>
+      <c r="V43" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U43" s="20">
-        <v>0</v>
-      </c>
-      <c r="V43" s="20">
-        <v>1</v>
-      </c>
-      <c r="W43" s="21">
+      <c r="W43" s="20">
+        <v>0</v>
+      </c>
+      <c r="X43" s="20">
+        <v>1</v>
+      </c>
+      <c r="Y43" s="21">
         <v>0.6</v>
       </c>
     </row>
-    <row r="44" spans="1:23" s="20" customFormat="1" ht="17.649999999999999">
+    <row r="44" spans="1:25" s="20" customFormat="1" ht="17.649999999999999">
       <c r="A44" s="19" t="s">
         <v>80</v>
       </c>
@@ -3747,32 +4026,38 @@
       <c r="K44" s="21">
         <v>0</v>
       </c>
-      <c r="N44" s="21">
-        <v>1</v>
-      </c>
-      <c r="O44" s="20">
-        <v>0</v>
+      <c r="L44" s="21">
+        <v>1</v>
+      </c>
+      <c r="M44" s="21">
+        <v>0.3</v>
       </c>
       <c r="P44" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q44" s="20">
+        <v>0</v>
+      </c>
+      <c r="R44" s="21">
         <v>2</v>
       </c>
-      <c r="Q44" s="21">
-        <v>0</v>
-      </c>
-      <c r="T44" s="13" t="s">
+      <c r="S44" s="21">
+        <v>0</v>
+      </c>
+      <c r="V44" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U44" s="20">
-        <v>0</v>
-      </c>
-      <c r="V44" s="20">
-        <v>1</v>
-      </c>
-      <c r="W44" s="21">
+      <c r="W44" s="20">
+        <v>0</v>
+      </c>
+      <c r="X44" s="20">
+        <v>1</v>
+      </c>
+      <c r="Y44" s="21">
         <v>0.6</v>
       </c>
     </row>
-    <row r="45" spans="1:23" s="20" customFormat="1" ht="17.649999999999999">
+    <row r="45" spans="1:25" s="20" customFormat="1" ht="17.649999999999999">
       <c r="A45" s="19" t="s">
         <v>81</v>
       </c>
@@ -3801,32 +4086,38 @@
       <c r="K45" s="21">
         <v>0</v>
       </c>
-      <c r="N45" s="21">
-        <v>1</v>
-      </c>
-      <c r="O45" s="20">
-        <v>0</v>
+      <c r="L45" s="21">
+        <v>1</v>
+      </c>
+      <c r="M45" s="21">
+        <v>0.3</v>
       </c>
       <c r="P45" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q45" s="20">
+        <v>0</v>
+      </c>
+      <c r="R45" s="21">
         <v>2</v>
       </c>
-      <c r="Q45" s="21">
-        <v>0</v>
-      </c>
-      <c r="T45" s="13" t="s">
+      <c r="S45" s="21">
+        <v>0</v>
+      </c>
+      <c r="V45" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U45" s="20">
-        <v>0</v>
-      </c>
-      <c r="V45" s="20">
-        <v>1</v>
-      </c>
-      <c r="W45" s="21">
+      <c r="W45" s="20">
+        <v>0</v>
+      </c>
+      <c r="X45" s="20">
+        <v>1</v>
+      </c>
+      <c r="Y45" s="21">
         <v>0.6</v>
       </c>
     </row>
-    <row r="46" spans="1:23" s="20" customFormat="1" ht="17.649999999999999">
+    <row r="46" spans="1:25" s="20" customFormat="1" ht="17.649999999999999">
       <c r="A46" s="19" t="s">
         <v>82</v>
       </c>
@@ -3855,36 +4146,42 @@
       <c r="K46" s="21">
         <v>0</v>
       </c>
-      <c r="N46" s="21">
-        <v>1</v>
-      </c>
-      <c r="O46" s="20">
-        <v>0</v>
+      <c r="L46" s="21">
+        <v>1</v>
+      </c>
+      <c r="M46" s="21">
+        <v>0.3</v>
       </c>
       <c r="P46" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q46" s="20">
+        <v>0</v>
+      </c>
+      <c r="R46" s="21">
         <v>2</v>
       </c>
-      <c r="Q46" s="21">
-        <v>0</v>
-      </c>
-      <c r="T46" s="13" t="s">
+      <c r="S46" s="21">
+        <v>0</v>
+      </c>
+      <c r="V46" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="U46" s="20">
-        <v>0</v>
-      </c>
-      <c r="V46" s="20">
-        <v>1</v>
-      </c>
-      <c r="W46" s="21">
+      <c r="W46" s="20">
+        <v>0</v>
+      </c>
+      <c r="X46" s="20">
+        <v>1</v>
+      </c>
+      <c r="Y46" s="21">
         <v>0.6</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:X9">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:Z9" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fixed bug for login module: it will always successful when both the account and password are empty string.
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Skill.xlsx
+++ b/_Out/NFDataCfg/Excel/Skill.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135">
   <si>
     <t>Id</t>
   </si>
@@ -251,9 +251,6 @@
     <t>SKILL_Dwarf_Warrior_Normal</t>
   </si>
   <si>
-    <t>NormalSkill1,NormalSkill2,NormalSkill4</t>
-  </si>
-  <si>
     <t>skill2</t>
   </si>
   <si>
@@ -263,70 +260,49 @@
     <t>SKILL_Wererat_Soldier_Normal</t>
   </si>
   <si>
-    <t>NormalSkill1,NormalSkill2,NormalSkill5</t>
-  </si>
-  <si>
     <t>skill3</t>
   </si>
   <si>
     <t>SKILL_Bristleback_Normal</t>
   </si>
   <si>
-    <t>NormalSkill1,NormalSkill2,NormalSkill6</t>
-  </si>
-  <si>
     <t>skill4</t>
   </si>
   <si>
     <t>SKILL_Clinkz_Normal</t>
   </si>
   <si>
-    <t>NormalSkill1,NormalSkill2,NormalSkill7</t>
-  </si>
-  <si>
     <t>skill5</t>
   </si>
   <si>
     <t>SKILL_CrystalMaiden_Normal</t>
   </si>
   <si>
-    <t>NormalSkill1,NormalSkill2,NormalSkill8</t>
-  </si>
-  <si>
     <t>skill6</t>
   </si>
   <si>
     <t>SKILL_Ezalor_Normal</t>
   </si>
   <si>
-    <t>NormalSkill1,NormalSkill2,NormalSkill9</t>
-  </si>
-  <si>
     <t>skill7</t>
   </si>
   <si>
     <t>SKILL_Lifestealer_Normal</t>
   </si>
   <si>
-    <t>NormalSkill1,NormalSkill2,NormalSkill10</t>
-  </si>
-  <si>
     <t>skill8</t>
   </si>
   <si>
     <t>SKILL_TeaantProtector_Normal</t>
   </si>
   <si>
-    <t>NormalSkill1,NormalSkill2,NormalSkill11</t>
-  </si>
-  <si>
     <t>skill9</t>
   </si>
   <si>
     <t>SKILL_Orc_Slinger_Attack</t>
   </si>
   <si>
-    <t>SpecialAttack1</t>
+    <t>SpecialSkill1</t>
   </si>
   <si>
     <t>club_crushing_blow_1</t>
@@ -365,7 +341,7 @@
     <t>SKILL_Orc_Slinger_THUMP</t>
   </si>
   <si>
-    <t>SpecialAttack2</t>
+    <t>SpecialSkill2</t>
   </si>
   <si>
     <t>strengthening</t>
@@ -479,9 +455,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -541,20 +517,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -574,25 +542,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -601,6 +554,14 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -644,10 +605,33 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -658,8 +642,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -673,17 +658,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -818,7 +794,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -830,13 +866,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -848,55 +896,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -908,25 +914,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -938,31 +932,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1064,20 +1040,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1106,17 +1086,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1136,6 +1110,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1150,162 +1135,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="38" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1871,9 +1847,9 @@
   <dimension ref="A1:Z61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="10" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
+      <selection pane="bottomLeft" activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2774,10 +2750,10 @@
         <v>0</v>
       </c>
       <c r="C12" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="25" t="s">
         <v>69</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>70</v>
       </c>
       <c r="E12" s="24"/>
       <c r="F12" s="24" t="s">
@@ -2830,21 +2806,21 @@
         <v>1</v>
       </c>
       <c r="Y12" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" s="5" customFormat="1" spans="1:25">
       <c r="A13" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="25" t="s">
         <v>72</v>
-      </c>
-      <c r="B13" s="5">
-        <v>0</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>74</v>
       </c>
       <c r="E13" s="24"/>
       <c r="F13" s="24" t="s">
@@ -2902,16 +2878,16 @@
     </row>
     <row r="14" s="5" customFormat="1" spans="1:25">
       <c r="A14" s="24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B14" s="5">
         <v>0</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E14" s="24"/>
       <c r="F14" s="24" t="s">
@@ -2969,16 +2945,16 @@
     </row>
     <row r="15" s="5" customFormat="1" spans="1:25">
       <c r="A15" s="24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B15" s="5">
         <v>0</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E15" s="24"/>
       <c r="F15" s="24" t="s">
@@ -3036,16 +3012,16 @@
     </row>
     <row r="16" s="5" customFormat="1" spans="1:25">
       <c r="A16" s="24" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B16" s="5">
         <v>0</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E16" s="24"/>
       <c r="F16" s="24" t="s">
@@ -3103,16 +3079,16 @@
     </row>
     <row r="17" s="5" customFormat="1" spans="1:25">
       <c r="A17" s="24" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B17" s="5">
         <v>0</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E17" s="24"/>
       <c r="F17" s="24" t="s">
@@ -3170,16 +3146,16 @@
     </row>
     <row r="18" s="5" customFormat="1" spans="1:25">
       <c r="A18" s="24" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B18" s="5">
         <v>0</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E18" s="24"/>
       <c r="F18" s="24" t="s">
@@ -3237,16 +3213,16 @@
     </row>
     <row r="19" s="5" customFormat="1" spans="1:25">
       <c r="A19" s="24" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B19" s="5">
         <v>0</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="E19" s="24"/>
       <c r="F19" s="24" t="s">
@@ -3304,13 +3280,13 @@
     </row>
     <row r="20" s="6" customFormat="1" spans="1:25">
       <c r="A20" s="26" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B20" s="6">
         <v>0</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F20" s="27" t="s">
         <v>64</v>
@@ -3349,7 +3325,7 @@
         <v>0</v>
       </c>
       <c r="U20" s="6" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="V20" s="24" t="s">
         <v>66</v>
@@ -3366,13 +3342,13 @@
     </row>
     <row r="21" s="6" customFormat="1" spans="1:25">
       <c r="A21" s="26" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B21" s="6">
         <v>0</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F21" s="27" t="s">
         <v>64</v>
@@ -3411,7 +3387,7 @@
         <v>0</v>
       </c>
       <c r="U21" s="6" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="V21" s="24" t="s">
         <v>66</v>
@@ -3428,13 +3404,13 @@
     </row>
     <row r="22" s="6" customFormat="1" spans="1:25">
       <c r="A22" s="26" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B22" s="6">
         <v>0</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F22" s="27" t="s">
         <v>64</v>
@@ -3473,7 +3449,7 @@
         <v>0</v>
       </c>
       <c r="U22" s="6" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="V22" s="24" t="s">
         <v>66</v>
@@ -3490,13 +3466,13 @@
     </row>
     <row r="23" s="6" customFormat="1" spans="1:25">
       <c r="A23" s="26" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B23" s="6">
         <v>0</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F23" s="27" t="s">
         <v>64</v>
@@ -3549,13 +3525,13 @@
     </row>
     <row r="24" s="6" customFormat="1" spans="1:25">
       <c r="A24" s="26" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B24" s="6">
         <v>0</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F24" s="27" t="s">
         <v>64</v>
@@ -3608,13 +3584,13 @@
     </row>
     <row r="25" s="6" customFormat="1" spans="1:25">
       <c r="A25" s="26" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B25" s="6">
         <v>0</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F25" s="27" t="s">
         <v>64</v>
@@ -3667,13 +3643,13 @@
     </row>
     <row r="26" s="6" customFormat="1" spans="1:25">
       <c r="A26" s="26" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B26" s="6">
         <v>0</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F26" s="27" t="s">
         <v>64</v>
@@ -3726,13 +3702,13 @@
     </row>
     <row r="27" s="6" customFormat="1" spans="1:25">
       <c r="A27" s="26" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B27" s="6">
         <v>0</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F27" s="27" t="s">
         <v>64</v>
@@ -3785,13 +3761,13 @@
     </row>
     <row r="28" s="6" customFormat="1" ht="15" customHeight="1" spans="1:25">
       <c r="A28" s="26" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B28" s="6">
         <v>0</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F28" s="27" t="s">
         <v>64</v>
@@ -3844,13 +3820,13 @@
     </row>
     <row r="29" s="7" customFormat="1" ht="18.75" spans="1:25">
       <c r="A29" s="28" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B29" s="7">
         <v>0</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D29" s="30"/>
       <c r="F29" s="31" t="s">
@@ -3890,7 +3866,7 @@
         <v>0</v>
       </c>
       <c r="U29" s="7" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="V29" s="24" t="s">
         <v>66</v>
@@ -3907,13 +3883,13 @@
     </row>
     <row r="30" s="7" customFormat="1" ht="18.75" spans="1:25">
       <c r="A30" s="28" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B30" s="7">
         <v>0</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D30" s="30"/>
       <c r="F30" s="31" t="s">
@@ -3953,7 +3929,7 @@
         <v>0</v>
       </c>
       <c r="U30" s="7" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="V30" s="24" t="s">
         <v>66</v>
@@ -3970,13 +3946,13 @@
     </row>
     <row r="31" s="7" customFormat="1" ht="18.75" spans="1:25">
       <c r="A31" s="28" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B31" s="7">
         <v>0</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D31" s="30"/>
       <c r="F31" s="31" t="s">
@@ -4016,7 +3992,7 @@
         <v>0</v>
       </c>
       <c r="U31" s="7" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="V31" s="24" t="s">
         <v>66</v>
@@ -4033,13 +4009,13 @@
     </row>
     <row r="32" s="7" customFormat="1" ht="18.75" spans="1:25">
       <c r="A32" s="28" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B32" s="7">
         <v>0</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D32" s="30"/>
       <c r="F32" s="31" t="s">
@@ -4093,13 +4069,13 @@
     </row>
     <row r="33" s="7" customFormat="1" ht="18.75" spans="1:25">
       <c r="A33" s="28" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B33" s="7">
         <v>0</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D33" s="30"/>
       <c r="F33" s="31" t="s">
@@ -4153,13 +4129,13 @@
     </row>
     <row r="34" s="7" customFormat="1" ht="18.75" spans="1:25">
       <c r="A34" s="28" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B34" s="7">
         <v>0</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D34" s="30"/>
       <c r="F34" s="31" t="s">
@@ -4213,13 +4189,13 @@
     </row>
     <row r="35" s="7" customFormat="1" ht="18.75" spans="1:25">
       <c r="A35" s="28" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B35" s="7">
         <v>0</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D35" s="30"/>
       <c r="F35" s="31" t="s">
@@ -4273,13 +4249,13 @@
     </row>
     <row r="36" s="7" customFormat="1" ht="18.75" spans="1:25">
       <c r="A36" s="28" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B36" s="7">
         <v>0</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D36" s="30"/>
       <c r="F36" s="31" t="s">
@@ -4333,13 +4309,13 @@
     </row>
     <row r="37" s="7" customFormat="1" ht="18.75" spans="1:25">
       <c r="A37" s="28" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B37" s="7">
         <v>0</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D37" s="30"/>
       <c r="F37" s="31" t="s">
@@ -4393,7 +4369,7 @@
     </row>
     <row r="38" s="8" customFormat="1" spans="1:25">
       <c r="A38" s="8" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B38" s="8">
         <v>0</v>
@@ -4444,13 +4420,13 @@
     </row>
     <row r="39" s="8" customFormat="1" spans="1:25">
       <c r="A39" s="8" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B39" s="8">
         <v>0</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="H39" s="8">
         <v>0</v>
@@ -4494,13 +4470,13 @@
     </row>
     <row r="40" s="8" customFormat="1" ht="18.75" spans="1:25">
       <c r="A40" s="8" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B40" s="8">
         <v>0</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D40" s="33"/>
       <c r="H40" s="8">
@@ -4545,7 +4521,7 @@
     </row>
     <row r="41" s="9" customFormat="1" spans="1:25">
       <c r="A41" s="9" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B41" s="9">
         <v>0</v>
@@ -4596,13 +4572,13 @@
     </row>
     <row r="42" s="9" customFormat="1" spans="1:25">
       <c r="A42" s="9" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B42" s="9">
         <v>0</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="H42" s="9">
         <v>0</v>
@@ -4646,13 +4622,13 @@
     </row>
     <row r="43" s="9" customFormat="1" ht="18.75" spans="1:25">
       <c r="A43" s="9" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B43" s="9">
         <v>0</v>
       </c>
       <c r="C43" s="35" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D43" s="35"/>
       <c r="H43" s="9">
@@ -4697,7 +4673,7 @@
     </row>
     <row r="44" s="10" customFormat="1" spans="1:25">
       <c r="A44" s="10" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B44" s="10">
         <v>0</v>
@@ -4748,13 +4724,13 @@
     </row>
     <row r="45" s="10" customFormat="1" spans="1:25">
       <c r="A45" s="10" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B45" s="10">
         <v>0</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="H45" s="10">
         <v>0</v>
@@ -4798,13 +4774,13 @@
     </row>
     <row r="46" s="10" customFormat="1" ht="18.75" spans="1:25">
       <c r="A46" s="10" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B46" s="10">
         <v>0</v>
       </c>
       <c r="C46" s="37" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D46" s="37"/>
       <c r="H46" s="10">
@@ -4849,7 +4825,7 @@
     </row>
     <row r="47" s="11" customFormat="1" spans="1:25">
       <c r="A47" s="11" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B47" s="11">
         <v>0</v>
@@ -4900,13 +4876,13 @@
     </row>
     <row r="48" s="11" customFormat="1" spans="1:25">
       <c r="A48" s="11" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B48" s="11">
         <v>0</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="H48" s="11">
         <v>0</v>
@@ -4950,13 +4926,13 @@
     </row>
     <row r="49" s="11" customFormat="1" ht="18.75" spans="1:25">
       <c r="A49" s="11" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B49" s="11">
         <v>0</v>
       </c>
       <c r="C49" s="39" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D49" s="39"/>
       <c r="H49" s="11">
@@ -5001,7 +4977,7 @@
     </row>
     <row r="50" s="12" customFormat="1" spans="1:25">
       <c r="A50" s="12" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B50" s="12">
         <v>0</v>
@@ -5052,13 +5028,13 @@
     </row>
     <row r="51" s="12" customFormat="1" spans="1:25">
       <c r="A51" s="12" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B51" s="12">
         <v>0</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="H51" s="12">
         <v>0</v>
@@ -5102,13 +5078,13 @@
     </row>
     <row r="52" s="12" customFormat="1" ht="18.75" spans="1:25">
       <c r="A52" s="12" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B52" s="12">
         <v>0</v>
       </c>
       <c r="C52" s="41" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D52" s="41"/>
       <c r="H52" s="12">
@@ -5153,7 +5129,7 @@
     </row>
     <row r="53" s="13" customFormat="1" spans="1:25">
       <c r="A53" s="13" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B53" s="13">
         <v>0</v>
@@ -5204,13 +5180,13 @@
     </row>
     <row r="54" s="13" customFormat="1" spans="1:25">
       <c r="A54" s="13" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B54" s="13">
         <v>0</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="H54" s="13">
         <v>0</v>
@@ -5254,13 +5230,13 @@
     </row>
     <row r="55" s="13" customFormat="1" ht="18.75" spans="1:25">
       <c r="A55" s="13" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B55" s="13">
         <v>0</v>
       </c>
       <c r="C55" s="43" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D55" s="43"/>
       <c r="H55" s="13">
@@ -5305,7 +5281,7 @@
     </row>
     <row r="56" s="14" customFormat="1" spans="1:25">
       <c r="A56" s="14" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B56" s="14">
         <v>0</v>
@@ -5356,13 +5332,13 @@
     </row>
     <row r="57" s="14" customFormat="1" spans="1:25">
       <c r="A57" s="14" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B57" s="14">
         <v>0</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="H57" s="14">
         <v>0</v>
@@ -5406,13 +5382,13 @@
     </row>
     <row r="58" s="14" customFormat="1" ht="18.75" spans="1:25">
       <c r="A58" s="14" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B58" s="14">
         <v>0</v>
       </c>
       <c r="C58" s="45" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D58" s="45"/>
       <c r="H58" s="14">
@@ -5457,7 +5433,7 @@
     </row>
     <row r="59" s="15" customFormat="1" spans="1:25">
       <c r="A59" s="15" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B59" s="15">
         <v>0</v>
@@ -5508,13 +5484,13 @@
     </row>
     <row r="60" s="15" customFormat="1" spans="1:25">
       <c r="A60" s="15" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B60" s="15">
         <v>0</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="H60" s="15">
         <v>0</v>
@@ -5558,13 +5534,13 @@
     </row>
     <row r="61" s="15" customFormat="1" ht="18.75" spans="1:25">
       <c r="A61" s="15" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B61" s="15">
         <v>0</v>
       </c>
       <c r="C61" s="47" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D61" s="47"/>
       <c r="H61" s="15">

</xml_diff>

<commit_message>
position sync create a building by player's position
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Skill.xlsx
+++ b/_Out/NFDataCfg/Excel/Skill.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/James/Desktop/ctc/Excel/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="18405" windowHeight="8115"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27980" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -13,13 +18,21 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Property1!$C$11:$C$19</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Skill" type="4" background="1" refreshedVersion="2" saveData="1">
-    <webPr parsePre="1" consecutive="1" xl2000="1" sourceData="1" xml="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\Skill.xml" htmlFormat="all" htmlTables="1"/>
+  <connection id="1" name="Skill" type="4" refreshedVersion="2" background="1" saveData="1">
+    <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\Skill.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
@@ -452,14 +465,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="29">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -513,159 +520,8 @@
       <name val="宋体"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="47">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -692,13 +548,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.599993896298105"/>
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -710,31 +566,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.349986266670736"/>
+        <fgColor theme="1" tint="0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -752,198 +608,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.4"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.6"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.4"/>
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.35"/>
+        <fgColor theme="1" tint="0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.05"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="-0.25"/>
+        <fgColor theme="6" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1037,251 +743,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="33" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1455,57 +919,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1838,46 +1255,45 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="Y61" sqref="Y61"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R61" sqref="R61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="49.5" customWidth="1"/>
-    <col min="3" max="3" width="43.75" customWidth="1"/>
-    <col min="4" max="5" width="18.8333333333333" customWidth="1"/>
+    <col min="3" max="3" width="43.6640625" customWidth="1"/>
+    <col min="4" max="5" width="18.83203125" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="15.3333333333333" customWidth="1"/>
-    <col min="8" max="8" width="17.6666666666667" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
     <col min="9" max="13" width="20" customWidth="1"/>
-    <col min="14" max="14" width="17.1666666666667" customWidth="1"/>
-    <col min="15" max="15" width="21.1666666666667" customWidth="1"/>
-    <col min="16" max="16" width="13.6666666666667" customWidth="1"/>
-    <col min="17" max="17" width="16.8333333333333" customWidth="1"/>
+    <col min="14" max="14" width="17.1640625" customWidth="1"/>
+    <col min="15" max="15" width="21.1640625" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" customWidth="1"/>
+    <col min="17" max="17" width="16.83203125" customWidth="1"/>
     <col min="18" max="18" width="19" customWidth="1"/>
-    <col min="19" max="19" width="26.3333333333333" customWidth="1"/>
+    <col min="19" max="19" width="26.33203125" customWidth="1"/>
     <col min="20" max="20" width="19" customWidth="1"/>
     <col min="21" max="21" width="19.5" customWidth="1"/>
-    <col min="22" max="22" width="42.3333333333333" customWidth="1"/>
+    <col min="22" max="22" width="42.33203125" customWidth="1"/>
     <col min="23" max="23" width="16.5" customWidth="1"/>
     <col min="24" max="24" width="23" customWidth="1"/>
-    <col min="25" max="25" width="23.1666666666667" customWidth="1"/>
+    <col min="25" max="25" width="23.1640625" customWidth="1"/>
     <col min="26" max="26" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:26">
+    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1957,7 +1373,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="1" spans="1:26">
+    <row r="2" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="18" t="s">
         <v>26</v>
       </c>
@@ -2037,7 +1453,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="1" spans="1:26">
+    <row r="3" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="18" t="s">
         <v>30</v>
       </c>
@@ -2117,7 +1533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" s="2" customFormat="1" spans="1:26">
+    <row r="4" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="18" t="s">
         <v>31</v>
       </c>
@@ -2197,7 +1613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" s="2" customFormat="1" spans="1:26">
+    <row r="5" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="18" t="s">
         <v>32</v>
       </c>
@@ -2277,7 +1693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" s="2" customFormat="1" spans="1:26">
+    <row r="6" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="18" t="s">
         <v>33</v>
       </c>
@@ -2357,7 +1773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" spans="1:26">
+    <row r="7" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="20" t="s">
         <v>34</v>
       </c>
@@ -2437,7 +1853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" s="3" customFormat="1" spans="1:26">
+    <row r="8" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="20" t="s">
         <v>35</v>
       </c>
@@ -2517,7 +1933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" s="3" customFormat="1" spans="1:26">
+    <row r="9" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="20" t="s">
         <v>36</v>
       </c>
@@ -2597,7 +2013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" s="4" customFormat="1" ht="17" customHeight="1" spans="1:26">
+    <row r="10" spans="1:26" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="22" t="s">
         <v>4</v>
       </c>
@@ -2675,7 +2091,7 @@
       </c>
       <c r="Z10" s="23"/>
     </row>
-    <row r="11" s="5" customFormat="1" spans="1:25">
+    <row r="11" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A11" s="24" t="s">
         <v>61</v>
       </c>
@@ -2716,13 +2132,13 @@
       <c r="N11" s="24"/>
       <c r="O11" s="24"/>
       <c r="P11" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q11" s="24">
         <v>0</v>
       </c>
       <c r="R11" s="24">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S11" s="24">
         <v>0</v>
@@ -2742,7 +2158,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" s="5" customFormat="1" spans="1:25">
+    <row r="12" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="24" t="s">
         <v>68</v>
       </c>
@@ -2783,13 +2199,13 @@
       <c r="N12" s="24"/>
       <c r="O12" s="24"/>
       <c r="P12" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q12" s="24">
         <v>0</v>
       </c>
       <c r="R12" s="24">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S12" s="24">
         <v>0</v>
@@ -2809,7 +2225,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" s="5" customFormat="1" spans="1:25">
+    <row r="13" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="24" t="s">
         <v>71</v>
       </c>
@@ -2850,13 +2266,13 @@
       <c r="N13" s="24"/>
       <c r="O13" s="24"/>
       <c r="P13" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q13" s="24">
         <v>0</v>
       </c>
       <c r="R13" s="24">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S13" s="24">
         <v>0</v>
@@ -2876,7 +2292,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" s="5" customFormat="1" spans="1:25">
+    <row r="14" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="24" t="s">
         <v>73</v>
       </c>
@@ -2917,13 +2333,13 @@
       <c r="N14" s="24"/>
       <c r="O14" s="24"/>
       <c r="P14" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q14" s="24">
         <v>0</v>
       </c>
       <c r="R14" s="24">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S14" s="24">
         <v>0</v>
@@ -2943,7 +2359,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" s="5" customFormat="1" spans="1:25">
+    <row r="15" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A15" s="24" t="s">
         <v>75</v>
       </c>
@@ -2984,13 +2400,13 @@
       <c r="N15" s="24"/>
       <c r="O15" s="24"/>
       <c r="P15" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q15" s="24">
         <v>0</v>
       </c>
       <c r="R15" s="24">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S15" s="24">
         <v>0</v>
@@ -3010,7 +2426,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" s="5" customFormat="1" spans="1:25">
+    <row r="16" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A16" s="24" t="s">
         <v>77</v>
       </c>
@@ -3051,13 +2467,13 @@
       <c r="N16" s="24"/>
       <c r="O16" s="24"/>
       <c r="P16" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q16" s="24">
         <v>0</v>
       </c>
       <c r="R16" s="24">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S16" s="24">
         <v>0</v>
@@ -3077,7 +2493,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" s="5" customFormat="1" spans="1:25">
+    <row r="17" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A17" s="24" t="s">
         <v>79</v>
       </c>
@@ -3118,13 +2534,13 @@
       <c r="N17" s="24"/>
       <c r="O17" s="24"/>
       <c r="P17" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="24">
         <v>0</v>
       </c>
       <c r="R17" s="24">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S17" s="24">
         <v>0</v>
@@ -3144,7 +2560,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" s="5" customFormat="1" spans="1:25">
+    <row r="18" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A18" s="24" t="s">
         <v>81</v>
       </c>
@@ -3185,13 +2601,13 @@
       <c r="N18" s="24"/>
       <c r="O18" s="24"/>
       <c r="P18" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q18" s="24">
         <v>0</v>
       </c>
       <c r="R18" s="24">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S18" s="24">
         <v>0</v>
@@ -3211,7 +2627,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" s="5" customFormat="1" spans="1:25">
+    <row r="19" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A19" s="24" t="s">
         <v>83</v>
       </c>
@@ -3252,13 +2668,13 @@
       <c r="N19" s="24"/>
       <c r="O19" s="24"/>
       <c r="P19" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q19" s="24">
         <v>0</v>
       </c>
       <c r="R19" s="24">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S19" s="24">
         <v>0</v>
@@ -3278,7 +2694,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" s="6" customFormat="1" spans="1:25">
+    <row r="20" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A20" s="26" t="s">
         <v>85</v>
       </c>
@@ -3319,7 +2735,7 @@
         <v>0</v>
       </c>
       <c r="R20" s="27">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S20" s="27">
         <v>0</v>
@@ -3340,7 +2756,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="21" s="6" customFormat="1" spans="1:25">
+    <row r="21" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="26" t="s">
         <v>88</v>
       </c>
@@ -3381,7 +2797,7 @@
         <v>0</v>
       </c>
       <c r="R21" s="27">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S21" s="27">
         <v>0</v>
@@ -3402,7 +2818,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="22" s="6" customFormat="1" spans="1:25">
+    <row r="22" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A22" s="26" t="s">
         <v>90</v>
       </c>
@@ -3443,7 +2859,7 @@
         <v>0</v>
       </c>
       <c r="R22" s="27">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S22" s="27">
         <v>0</v>
@@ -3464,7 +2880,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="23" s="6" customFormat="1" spans="1:25">
+    <row r="23" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A23" s="26" t="s">
         <v>92</v>
       </c>
@@ -3505,7 +2921,7 @@
         <v>0</v>
       </c>
       <c r="R23" s="27">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S23" s="27">
         <v>0</v>
@@ -3523,7 +2939,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="24" s="6" customFormat="1" spans="1:25">
+    <row r="24" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A24" s="26" t="s">
         <v>93</v>
       </c>
@@ -3564,7 +2980,7 @@
         <v>0</v>
       </c>
       <c r="R24" s="27">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S24" s="27">
         <v>0</v>
@@ -3582,7 +2998,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="25" s="6" customFormat="1" spans="1:25">
+    <row r="25" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
         <v>94</v>
       </c>
@@ -3623,7 +3039,7 @@
         <v>0</v>
       </c>
       <c r="R25" s="27">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S25" s="27">
         <v>0</v>
@@ -3641,7 +3057,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="26" s="6" customFormat="1" spans="1:25">
+    <row r="26" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A26" s="26" t="s">
         <v>95</v>
       </c>
@@ -3682,7 +3098,7 @@
         <v>0</v>
       </c>
       <c r="R26" s="27">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S26" s="27">
         <v>0</v>
@@ -3700,7 +3116,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="27" s="6" customFormat="1" spans="1:25">
+    <row r="27" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A27" s="26" t="s">
         <v>96</v>
       </c>
@@ -3741,7 +3157,7 @@
         <v>0</v>
       </c>
       <c r="R27" s="27">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S27" s="27">
         <v>0</v>
@@ -3759,7 +3175,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="28" s="6" customFormat="1" ht="15" customHeight="1" spans="1:25">
+    <row r="28" spans="1:25" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="26" t="s">
         <v>97</v>
       </c>
@@ -3800,7 +3216,7 @@
         <v>0</v>
       </c>
       <c r="R28" s="27">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S28" s="27">
         <v>0</v>
@@ -3818,7 +3234,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="29" s="7" customFormat="1" ht="18.75" spans="1:25">
+    <row r="29" spans="1:25" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A29" s="28" t="s">
         <v>98</v>
       </c>
@@ -3860,7 +3276,7 @@
         <v>0</v>
       </c>
       <c r="R29" s="31">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S29" s="31">
         <v>0</v>
@@ -3881,7 +3297,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="30" s="7" customFormat="1" ht="18.75" spans="1:25">
+    <row r="30" spans="1:25" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" s="28" t="s">
         <v>101</v>
       </c>
@@ -3923,7 +3339,7 @@
         <v>0</v>
       </c>
       <c r="R30" s="31">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S30" s="31">
         <v>0</v>
@@ -3944,7 +3360,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="31" s="7" customFormat="1" ht="18.75" spans="1:25">
+    <row r="31" spans="1:25" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" s="28" t="s">
         <v>103</v>
       </c>
@@ -3986,7 +3402,7 @@
         <v>0</v>
       </c>
       <c r="R31" s="31">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S31" s="31">
         <v>0</v>
@@ -4007,7 +3423,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="32" s="7" customFormat="1" ht="18.75" spans="1:25">
+    <row r="32" spans="1:25" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A32" s="28" t="s">
         <v>105</v>
       </c>
@@ -4049,7 +3465,7 @@
         <v>0</v>
       </c>
       <c r="R32" s="31">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S32" s="31">
         <v>0</v>
@@ -4067,7 +3483,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="33" s="7" customFormat="1" ht="18.75" spans="1:25">
+    <row r="33" spans="1:25" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" s="28" t="s">
         <v>106</v>
       </c>
@@ -4109,7 +3525,7 @@
         <v>0</v>
       </c>
       <c r="R33" s="31">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S33" s="31">
         <v>0</v>
@@ -4127,7 +3543,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="34" s="7" customFormat="1" ht="18.75" spans="1:25">
+    <row r="34" spans="1:25" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A34" s="28" t="s">
         <v>107</v>
       </c>
@@ -4169,7 +3585,7 @@
         <v>0</v>
       </c>
       <c r="R34" s="31">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S34" s="31">
         <v>0</v>
@@ -4187,7 +3603,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="35" s="7" customFormat="1" ht="18.75" spans="1:25">
+    <row r="35" spans="1:25" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A35" s="28" t="s">
         <v>108</v>
       </c>
@@ -4229,7 +3645,7 @@
         <v>0</v>
       </c>
       <c r="R35" s="31">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S35" s="31">
         <v>0</v>
@@ -4247,7 +3663,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="36" s="7" customFormat="1" ht="18.75" spans="1:25">
+    <row r="36" spans="1:25" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A36" s="28" t="s">
         <v>109</v>
       </c>
@@ -4289,7 +3705,7 @@
         <v>0</v>
       </c>
       <c r="R36" s="31">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S36" s="31">
         <v>0</v>
@@ -4307,7 +3723,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="37" s="7" customFormat="1" ht="18.75" spans="1:25">
+    <row r="37" spans="1:25" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A37" s="28" t="s">
         <v>110</v>
       </c>
@@ -4349,7 +3765,7 @@
         <v>0</v>
       </c>
       <c r="R37" s="31">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S37" s="31">
         <v>0</v>
@@ -4367,7 +3783,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="38" s="8" customFormat="1" spans="1:25">
+    <row r="38" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A38" s="8" t="s">
         <v>111</v>
       </c>
@@ -4397,13 +3813,13 @@
         <v>0.3</v>
       </c>
       <c r="P38" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q38" s="24">
         <v>0</v>
       </c>
       <c r="R38" s="8">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S38" s="8">
         <v>0</v>
@@ -4418,7 +3834,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" s="8" customFormat="1" spans="1:25">
+    <row r="39" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A39" s="8" t="s">
         <v>112</v>
       </c>
@@ -4453,7 +3869,7 @@
         <v>0</v>
       </c>
       <c r="R39" s="8">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S39" s="8">
         <v>0</v>
@@ -4468,7 +3884,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="40" s="8" customFormat="1" ht="18.75" spans="1:25">
+    <row r="40" spans="1:25" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A40" s="8" t="s">
         <v>113</v>
       </c>
@@ -4504,7 +3920,7 @@
         <v>0</v>
       </c>
       <c r="R40" s="8">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S40" s="8">
         <v>0</v>
@@ -4519,7 +3935,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="41" s="9" customFormat="1" spans="1:25">
+    <row r="41" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A41" s="9" t="s">
         <v>114</v>
       </c>
@@ -4549,13 +3965,13 @@
         <v>0.3</v>
       </c>
       <c r="P41" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q41" s="24">
         <v>0</v>
       </c>
       <c r="R41" s="9">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S41" s="9">
         <v>0</v>
@@ -4570,7 +3986,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" s="9" customFormat="1" spans="1:25">
+    <row r="42" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A42" s="9" t="s">
         <v>115</v>
       </c>
@@ -4605,7 +4021,7 @@
         <v>0</v>
       </c>
       <c r="R42" s="9">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S42" s="9">
         <v>0</v>
@@ -4620,7 +4036,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="43" s="9" customFormat="1" ht="18.75" spans="1:25">
+    <row r="43" spans="1:25" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A43" s="9" t="s">
         <v>116</v>
       </c>
@@ -4656,7 +4072,7 @@
         <v>0</v>
       </c>
       <c r="R43" s="9">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S43" s="9">
         <v>0</v>
@@ -4671,7 +4087,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="44" s="10" customFormat="1" spans="1:25">
+    <row r="44" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A44" s="10" t="s">
         <v>117</v>
       </c>
@@ -4707,7 +4123,7 @@
         <v>0</v>
       </c>
       <c r="R44" s="10">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S44" s="10">
         <v>0</v>
@@ -4722,7 +4138,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" s="10" customFormat="1" spans="1:25">
+    <row r="45" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A45" s="10" t="s">
         <v>118</v>
       </c>
@@ -4757,7 +4173,7 @@
         <v>0</v>
       </c>
       <c r="R45" s="10">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S45" s="10">
         <v>0</v>
@@ -4772,7 +4188,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="46" s="10" customFormat="1" ht="18.75" spans="1:25">
+    <row r="46" spans="1:25" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A46" s="10" t="s">
         <v>119</v>
       </c>
@@ -4808,7 +4224,7 @@
         <v>0</v>
       </c>
       <c r="R46" s="10">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S46" s="10">
         <v>0</v>
@@ -4823,7 +4239,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="47" s="11" customFormat="1" spans="1:25">
+    <row r="47" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A47" s="11" t="s">
         <v>120</v>
       </c>
@@ -4853,13 +4269,13 @@
         <v>0.3</v>
       </c>
       <c r="P47" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q47" s="24">
         <v>0</v>
       </c>
       <c r="R47" s="11">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S47" s="11">
         <v>0</v>
@@ -4874,7 +4290,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="48" s="11" customFormat="1" spans="1:25">
+    <row r="48" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A48" s="11" t="s">
         <v>121</v>
       </c>
@@ -4909,7 +4325,7 @@
         <v>0</v>
       </c>
       <c r="R48" s="11">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S48" s="11">
         <v>0</v>
@@ -4924,7 +4340,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="49" s="11" customFormat="1" ht="18.75" spans="1:25">
+    <row r="49" spans="1:25" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A49" s="11" t="s">
         <v>122</v>
       </c>
@@ -4960,7 +4376,7 @@
         <v>0</v>
       </c>
       <c r="R49" s="11">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S49" s="11">
         <v>0</v>
@@ -4975,7 +4391,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="50" s="12" customFormat="1" spans="1:25">
+    <row r="50" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A50" s="12" t="s">
         <v>123</v>
       </c>
@@ -5005,13 +4421,13 @@
         <v>0.3</v>
       </c>
       <c r="P50" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q50" s="24">
         <v>0</v>
       </c>
       <c r="R50" s="12">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S50" s="12">
         <v>0</v>
@@ -5026,7 +4442,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="51" s="12" customFormat="1" spans="1:25">
+    <row r="51" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A51" s="12" t="s">
         <v>124</v>
       </c>
@@ -5061,7 +4477,7 @@
         <v>0</v>
       </c>
       <c r="R51" s="12">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S51" s="12">
         <v>0</v>
@@ -5076,7 +4492,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="52" s="12" customFormat="1" ht="18.75" spans="1:25">
+    <row r="52" spans="1:25" s="12" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A52" s="12" t="s">
         <v>125</v>
       </c>
@@ -5112,7 +4528,7 @@
         <v>0</v>
       </c>
       <c r="R52" s="12">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S52" s="12">
         <v>0</v>
@@ -5127,7 +4543,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="53" s="13" customFormat="1" spans="1:25">
+    <row r="53" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A53" s="13" t="s">
         <v>126</v>
       </c>
@@ -5157,13 +4573,13 @@
         <v>0.3</v>
       </c>
       <c r="P53" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q53" s="24">
         <v>0</v>
       </c>
       <c r="R53" s="13">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S53" s="13">
         <v>0</v>
@@ -5178,7 +4594,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="54" s="13" customFormat="1" spans="1:25">
+    <row r="54" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A54" s="13" t="s">
         <v>127</v>
       </c>
@@ -5213,7 +4629,7 @@
         <v>0</v>
       </c>
       <c r="R54" s="13">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S54" s="13">
         <v>0</v>
@@ -5228,7 +4644,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="55" s="13" customFormat="1" ht="18.75" spans="1:25">
+    <row r="55" spans="1:25" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A55" s="13" t="s">
         <v>128</v>
       </c>
@@ -5264,7 +4680,7 @@
         <v>0</v>
       </c>
       <c r="R55" s="13">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S55" s="13">
         <v>0</v>
@@ -5279,7 +4695,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="56" s="14" customFormat="1" spans="1:25">
+    <row r="56" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A56" s="14" t="s">
         <v>129</v>
       </c>
@@ -5309,13 +4725,13 @@
         <v>0.3</v>
       </c>
       <c r="P56" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q56" s="24">
         <v>0</v>
       </c>
       <c r="R56" s="14">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S56" s="14">
         <v>0</v>
@@ -5330,7 +4746,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="57" s="14" customFormat="1" spans="1:25">
+    <row r="57" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A57" s="14" t="s">
         <v>130</v>
       </c>
@@ -5365,7 +4781,7 @@
         <v>0</v>
       </c>
       <c r="R57" s="14">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S57" s="14">
         <v>0</v>
@@ -5380,7 +4796,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="58" s="14" customFormat="1" ht="18.75" spans="1:25">
+    <row r="58" spans="1:25" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A58" s="14" t="s">
         <v>131</v>
       </c>
@@ -5416,7 +4832,7 @@
         <v>0</v>
       </c>
       <c r="R58" s="14">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S58" s="14">
         <v>0</v>
@@ -5431,7 +4847,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="59" s="15" customFormat="1" spans="1:25">
+    <row r="59" spans="1:25" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A59" s="15" t="s">
         <v>132</v>
       </c>
@@ -5461,13 +4877,13 @@
         <v>0.3</v>
       </c>
       <c r="P59" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q59" s="24">
         <v>0</v>
       </c>
       <c r="R59" s="15">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S59" s="15">
         <v>0</v>
@@ -5482,7 +4898,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="60" s="15" customFormat="1" spans="1:25">
+    <row r="60" spans="1:25" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A60" s="15" t="s">
         <v>133</v>
       </c>
@@ -5517,7 +4933,7 @@
         <v>0</v>
       </c>
       <c r="R60" s="15">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S60" s="15">
         <v>0</v>
@@ -5532,7 +4948,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="61" s="15" customFormat="1" ht="18.75" spans="1:25">
+    <row r="61" spans="1:25" s="15" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A61" s="15" t="s">
         <v>134</v>
       </c>
@@ -5568,7 +4984,7 @@
         <v>0</v>
       </c>
       <c r="R61" s="15">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S61" s="15">
         <v>0</v>
@@ -5590,7 +5006,7 @@
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>

<commit_message>
fix bugs for scene module (for normal scene it should only crate one group except base group) fix bugs for broadcast module
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Skill.xlsx
+++ b/_Out/NFDataCfg/Excel/Skill.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="7560" activeTab="1"/>
+    <workbookView windowHeight="23360"/>
   </bookViews>
   <sheets>
     <sheet name="Property_hero" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346">
   <si>
     <t>Id</t>
   </si>
@@ -1080,9 +1080,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="28">
@@ -1134,31 +1134,27 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1170,32 +1166,15 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1209,47 +1188,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1264,14 +1204,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1280,6 +1220,66 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1348,7 +1348,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1360,13 +1396,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1378,73 +1432,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1462,13 +1456,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1480,31 +1486,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1629,36 +1629,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1669,15 +1639,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1706,6 +1667,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1716,153 +1692,177 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="35" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1957,54 +1957,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
@@ -2342,39 +2342,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A68" sqref="A68:A86"/>
+      <selection pane="bottomLeft" activeCell="X49" sqref="X49:X86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="49.5" customWidth="1"/>
-    <col min="3" max="3" width="43.6666666666667" customWidth="1"/>
-    <col min="4" max="4" width="33.725" customWidth="1"/>
-    <col min="5" max="5" width="27.8666666666667" customWidth="1"/>
+    <col min="3" max="3" width="43.6634615384615" customWidth="1"/>
+    <col min="4" max="4" width="33.7211538461538" customWidth="1"/>
+    <col min="5" max="5" width="27.8653846153846" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="15.3333333333333" customWidth="1"/>
-    <col min="8" max="8" width="17.6666666666667" customWidth="1"/>
+    <col min="7" max="7" width="15.3365384615385" customWidth="1"/>
+    <col min="8" max="8" width="17.6634615384615" customWidth="1"/>
     <col min="9" max="13" width="20" customWidth="1"/>
-    <col min="14" max="14" width="17.1666666666667" customWidth="1"/>
-    <col min="15" max="15" width="21.1666666666667" customWidth="1"/>
-    <col min="16" max="16" width="13.6666666666667" customWidth="1"/>
-    <col min="17" max="17" width="16.8333333333333" customWidth="1"/>
+    <col min="14" max="14" width="17.1634615384615" customWidth="1"/>
+    <col min="15" max="15" width="21.1634615384615" customWidth="1"/>
+    <col min="16" max="16" width="13.6634615384615" customWidth="1"/>
+    <col min="17" max="17" width="16.8365384615385" customWidth="1"/>
     <col min="18" max="18" width="19" customWidth="1"/>
-    <col min="19" max="19" width="26.3333333333333" customWidth="1"/>
+    <col min="19" max="19" width="26.3365384615385" customWidth="1"/>
     <col min="20" max="20" width="19" customWidth="1"/>
     <col min="21" max="21" width="31.625" customWidth="1"/>
-    <col min="22" max="22" width="42.3333333333333" customWidth="1"/>
+    <col min="22" max="22" width="42.3365384615385" customWidth="1"/>
     <col min="23" max="23" width="16.5" customWidth="1"/>
     <col min="24" max="24" width="23" customWidth="1"/>
-    <col min="25" max="25" width="23.1666666666667" customWidth="1"/>
+    <col min="25" max="25" width="23.1634615384615" customWidth="1"/>
     <col min="26" max="26" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2858,7 +2858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" spans="1:26">
+    <row r="7" s="3" customFormat="1" ht="17" spans="1:26">
       <c r="A7" s="10" t="s">
         <v>34</v>
       </c>
@@ -2938,7 +2938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" s="3" customFormat="1" spans="1:26">
+    <row r="8" s="3" customFormat="1" ht="17" spans="1:26">
       <c r="A8" s="10" t="s">
         <v>35</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" s="3" customFormat="1" spans="1:26">
+    <row r="9" s="3" customFormat="1" ht="17" spans="1:26">
       <c r="A9" s="10" t="s">
         <v>36</v>
       </c>
@@ -3237,7 +3237,7 @@
         <v>0</v>
       </c>
       <c r="X11" s="14">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y11" s="14" t="s">
         <v>67</v>
@@ -3304,7 +3304,7 @@
         <v>0</v>
       </c>
       <c r="X12" s="14">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y12" s="14" t="s">
         <v>70</v>
@@ -3371,7 +3371,7 @@
         <v>0</v>
       </c>
       <c r="X13" s="14">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y13" s="14" t="s">
         <v>67</v>
@@ -3438,13 +3438,13 @@
         <v>0</v>
       </c>
       <c r="X14" s="14">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y14" s="14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" s="17" customFormat="1" spans="1:25">
+    <row r="15" s="17" customFormat="1" ht="17" spans="1:25">
       <c r="A15" s="14" t="s">
         <v>75</v>
       </c>
@@ -3505,13 +3505,13 @@
         <v>0</v>
       </c>
       <c r="X15" s="14">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y15" s="28" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" s="17" customFormat="1" spans="1:25">
+    <row r="16" s="17" customFormat="1" ht="17" spans="1:25">
       <c r="A16" s="14" t="s">
         <v>77</v>
       </c>
@@ -3572,13 +3572,13 @@
         <v>0</v>
       </c>
       <c r="X16" s="14">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y16" s="28" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" s="17" customFormat="1" spans="1:25">
+    <row r="17" s="17" customFormat="1" ht="17" spans="1:25">
       <c r="A17" s="14" t="s">
         <v>79</v>
       </c>
@@ -3639,13 +3639,13 @@
         <v>0</v>
       </c>
       <c r="X17" s="14">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y17" s="28" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="18" s="17" customFormat="1" spans="1:25">
+    <row r="18" s="17" customFormat="1" ht="17" spans="1:25">
       <c r="A18" s="14" t="s">
         <v>81</v>
       </c>
@@ -3706,13 +3706,13 @@
         <v>0</v>
       </c>
       <c r="X18" s="14">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y18" s="28" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="19" s="17" customFormat="1" spans="1:25">
+    <row r="19" s="17" customFormat="1" ht="17" spans="1:25">
       <c r="A19" s="14" t="s">
         <v>83</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>0</v>
       </c>
       <c r="X19" s="14">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y19" s="28" t="s">
         <v>67</v>
@@ -3840,7 +3840,7 @@
         <v>0</v>
       </c>
       <c r="X20" s="14">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y20" s="14" t="s">
         <v>67</v>
@@ -3907,7 +3907,7 @@
         <v>0</v>
       </c>
       <c r="X21" s="14">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y21" s="14" t="s">
         <v>70</v>
@@ -3974,7 +3974,7 @@
         <v>0</v>
       </c>
       <c r="X22" s="14">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y22" s="14" t="s">
         <v>67</v>
@@ -4041,13 +4041,13 @@
         <v>0</v>
       </c>
       <c r="X23" s="14">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y23" s="14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="24" s="17" customFormat="1" spans="1:25">
+    <row r="24" s="17" customFormat="1" ht="17" spans="1:25">
       <c r="A24" s="14" t="s">
         <v>93</v>
       </c>
@@ -4108,13 +4108,13 @@
         <v>0</v>
       </c>
       <c r="X24" s="14">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y24" s="28" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25" s="17" customFormat="1" spans="1:25">
+    <row r="25" s="17" customFormat="1" ht="17" spans="1:25">
       <c r="A25" s="14" t="s">
         <v>95</v>
       </c>
@@ -4175,13 +4175,13 @@
         <v>0</v>
       </c>
       <c r="X25" s="14">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y25" s="28" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="26" s="17" customFormat="1" spans="1:25">
+    <row r="26" s="17" customFormat="1" ht="17" spans="1:25">
       <c r="A26" s="14" t="s">
         <v>97</v>
       </c>
@@ -4242,13 +4242,13 @@
         <v>0</v>
       </c>
       <c r="X26" s="14">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y26" s="28" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" s="17" customFormat="1" spans="1:25">
+    <row r="27" s="17" customFormat="1" ht="17" spans="1:25">
       <c r="A27" s="14" t="s">
         <v>99</v>
       </c>
@@ -4309,13 +4309,13 @@
         <v>0</v>
       </c>
       <c r="X27" s="14">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y27" s="28" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="28" s="17" customFormat="1" spans="1:25">
+    <row r="28" s="17" customFormat="1" ht="17" spans="1:25">
       <c r="A28" s="14" t="s">
         <v>101</v>
       </c>
@@ -4376,13 +4376,13 @@
         <v>0</v>
       </c>
       <c r="X28" s="14">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y28" s="28" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="29" s="17" customFormat="1" spans="1:25">
+    <row r="29" s="17" customFormat="1" ht="17" spans="1:25">
       <c r="A29" s="14" t="s">
         <v>103</v>
       </c>
@@ -4443,13 +4443,13 @@
         <v>0</v>
       </c>
       <c r="X29" s="14">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y29" s="28" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="30" s="18" customFormat="1" spans="1:25">
+    <row r="30" s="18" customFormat="1" ht="17" spans="1:25">
       <c r="A30" s="22" t="s">
         <v>105</v>
       </c>
@@ -4511,13 +4511,13 @@
         <v>0</v>
       </c>
       <c r="X30" s="18">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y30" s="20">
         <v>0.6</v>
       </c>
     </row>
-    <row r="31" s="18" customFormat="1" spans="1:25">
+    <row r="31" s="18" customFormat="1" ht="17" spans="1:25">
       <c r="A31" s="22" t="s">
         <v>110</v>
       </c>
@@ -4579,13 +4579,13 @@
         <v>0</v>
       </c>
       <c r="X31" s="18">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y31" s="20">
         <v>0.6</v>
       </c>
     </row>
-    <row r="32" s="18" customFormat="1" spans="1:25">
+    <row r="32" s="18" customFormat="1" ht="17" spans="1:25">
       <c r="A32" s="22" t="s">
         <v>114</v>
       </c>
@@ -4647,13 +4647,13 @@
         <v>0</v>
       </c>
       <c r="X32" s="18">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y32" s="20">
         <v>0.6</v>
       </c>
     </row>
-    <row r="33" s="18" customFormat="1" spans="1:25">
+    <row r="33" s="18" customFormat="1" ht="17" spans="1:25">
       <c r="A33" s="22" t="s">
         <v>118</v>
       </c>
@@ -4715,13 +4715,13 @@
         <v>0</v>
       </c>
       <c r="X33" s="18">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y33" s="20">
         <v>0.6</v>
       </c>
     </row>
-    <row r="34" s="18" customFormat="1" spans="1:25">
+    <row r="34" s="18" customFormat="1" ht="17" spans="1:25">
       <c r="A34" s="22" t="s">
         <v>122</v>
       </c>
@@ -4783,13 +4783,13 @@
         <v>0</v>
       </c>
       <c r="X34" s="18">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y34" s="20">
         <v>0.6</v>
       </c>
     </row>
-    <row r="35" s="18" customFormat="1" spans="1:25">
+    <row r="35" s="18" customFormat="1" ht="17" spans="1:25">
       <c r="A35" s="22" t="s">
         <v>126</v>
       </c>
@@ -4851,13 +4851,13 @@
         <v>0</v>
       </c>
       <c r="X35" s="18">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y35" s="20">
         <v>0.6</v>
       </c>
     </row>
-    <row r="36" s="18" customFormat="1" spans="1:25">
+    <row r="36" s="18" customFormat="1" ht="17" spans="1:25">
       <c r="A36" s="22" t="s">
         <v>130</v>
       </c>
@@ -4919,13 +4919,13 @@
         <v>0</v>
       </c>
       <c r="X36" s="18">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y36" s="20">
         <v>0.6</v>
       </c>
     </row>
-    <row r="37" s="18" customFormat="1" spans="1:25">
+    <row r="37" s="18" customFormat="1" ht="17" spans="1:25">
       <c r="A37" s="22" t="s">
         <v>134</v>
       </c>
@@ -4987,7 +4987,7 @@
         <v>0</v>
       </c>
       <c r="X37" s="18">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y37" s="20">
         <v>0.6</v>
@@ -5055,13 +5055,13 @@
         <v>0</v>
       </c>
       <c r="X38" s="18">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y38" s="20">
         <v>0.6</v>
       </c>
     </row>
-    <row r="39" s="18" customFormat="1" spans="1:25">
+    <row r="39" s="18" customFormat="1" ht="17" spans="1:25">
       <c r="A39" s="22" t="s">
         <v>142</v>
       </c>
@@ -5123,13 +5123,13 @@
         <v>0</v>
       </c>
       <c r="X39" s="18">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y39" s="20">
         <v>0.6</v>
       </c>
     </row>
-    <row r="40" s="18" customFormat="1" spans="1:25">
+    <row r="40" s="18" customFormat="1" ht="17" spans="1:25">
       <c r="A40" s="22" t="s">
         <v>146</v>
       </c>
@@ -5191,13 +5191,13 @@
         <v>0</v>
       </c>
       <c r="X40" s="18">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y40" s="20">
         <v>0.6</v>
       </c>
     </row>
-    <row r="41" s="18" customFormat="1" spans="1:25">
+    <row r="41" s="18" customFormat="1" ht="17" spans="1:25">
       <c r="A41" s="22" t="s">
         <v>150</v>
       </c>
@@ -5259,13 +5259,13 @@
         <v>0</v>
       </c>
       <c r="X41" s="18">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y41" s="20">
         <v>0.6</v>
       </c>
     </row>
-    <row r="42" s="18" customFormat="1" spans="1:25">
+    <row r="42" s="18" customFormat="1" ht="17" spans="1:25">
       <c r="A42" s="22" t="s">
         <v>154</v>
       </c>
@@ -5327,13 +5327,13 @@
         <v>0</v>
       </c>
       <c r="X42" s="18">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y42" s="20">
         <v>0.6</v>
       </c>
     </row>
-    <row r="43" s="18" customFormat="1" spans="1:25">
+    <row r="43" s="18" customFormat="1" ht="17" spans="1:25">
       <c r="A43" s="22" t="s">
         <v>158</v>
       </c>
@@ -5395,13 +5395,13 @@
         <v>0</v>
       </c>
       <c r="X43" s="18">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y43" s="20">
         <v>0.6</v>
       </c>
     </row>
-    <row r="44" s="18" customFormat="1" spans="1:25">
+    <row r="44" s="18" customFormat="1" ht="17" spans="1:25">
       <c r="A44" s="22" t="s">
         <v>162</v>
       </c>
@@ -5463,13 +5463,13 @@
         <v>0</v>
       </c>
       <c r="X44" s="18">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y44" s="20">
         <v>0.6</v>
       </c>
     </row>
-    <row r="45" s="18" customFormat="1" spans="1:25">
+    <row r="45" s="18" customFormat="1" ht="17" spans="1:25">
       <c r="A45" s="22" t="s">
         <v>166</v>
       </c>
@@ -5531,13 +5531,13 @@
         <v>0</v>
       </c>
       <c r="X45" s="18">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y45" s="20">
         <v>0.6</v>
       </c>
     </row>
-    <row r="46" s="18" customFormat="1" spans="1:25">
+    <row r="46" s="18" customFormat="1" ht="17" spans="1:25">
       <c r="A46" s="22" t="s">
         <v>170</v>
       </c>
@@ -5599,7 +5599,7 @@
         <v>0</v>
       </c>
       <c r="X46" s="18">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y46" s="20">
         <v>0.6</v>
@@ -5667,7 +5667,7 @@
         <v>0</v>
       </c>
       <c r="X47" s="18">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y47" s="20">
         <v>0.6</v>
@@ -5735,13 +5735,13 @@
         <v>0</v>
       </c>
       <c r="X48" s="18">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y48" s="20">
         <v>0.6</v>
       </c>
     </row>
-    <row r="49" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="49" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A49" s="24" t="s">
         <v>182</v>
       </c>
@@ -5803,13 +5803,13 @@
         <v>0</v>
       </c>
       <c r="X49" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y49" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="50" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="50" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A50" s="24" t="s">
         <v>187</v>
       </c>
@@ -5871,13 +5871,13 @@
         <v>0</v>
       </c>
       <c r="X50" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y50" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="51" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="51" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A51" s="24" t="s">
         <v>191</v>
       </c>
@@ -5939,13 +5939,13 @@
         <v>0</v>
       </c>
       <c r="X51" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y51" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="52" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="52" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A52" s="24" t="s">
         <v>195</v>
       </c>
@@ -6007,13 +6007,13 @@
         <v>0</v>
       </c>
       <c r="X52" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y52" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="53" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="53" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A53" s="24" t="s">
         <v>199</v>
       </c>
@@ -6075,13 +6075,13 @@
         <v>0</v>
       </c>
       <c r="X53" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y53" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="54" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="54" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A54" s="24" t="s">
         <v>203</v>
       </c>
@@ -6143,13 +6143,13 @@
         <v>0</v>
       </c>
       <c r="X54" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y54" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="55" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="55" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A55" s="24" t="s">
         <v>207</v>
       </c>
@@ -6211,13 +6211,13 @@
         <v>0</v>
       </c>
       <c r="X55" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y55" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="56" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="56" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A56" s="24" t="s">
         <v>211</v>
       </c>
@@ -6279,13 +6279,13 @@
         <v>0</v>
       </c>
       <c r="X56" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y56" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="57" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="57" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A57" s="24" t="s">
         <v>215</v>
       </c>
@@ -6347,13 +6347,13 @@
         <v>0</v>
       </c>
       <c r="X57" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y57" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="58" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="58" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A58" s="24" t="s">
         <v>219</v>
       </c>
@@ -6415,13 +6415,13 @@
         <v>0</v>
       </c>
       <c r="X58" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y58" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="59" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="59" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A59" s="24" t="s">
         <v>223</v>
       </c>
@@ -6483,13 +6483,13 @@
         <v>0</v>
       </c>
       <c r="X59" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y59" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="60" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="60" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A60" s="24" t="s">
         <v>227</v>
       </c>
@@ -6551,13 +6551,13 @@
         <v>0</v>
       </c>
       <c r="X60" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y60" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="61" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="61" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A61" s="24" t="s">
         <v>231</v>
       </c>
@@ -6619,13 +6619,13 @@
         <v>0</v>
       </c>
       <c r="X61" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y61" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="62" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="62" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A62" s="24" t="s">
         <v>235</v>
       </c>
@@ -6687,13 +6687,13 @@
         <v>0</v>
       </c>
       <c r="X62" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y62" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="63" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="63" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A63" s="24" t="s">
         <v>239</v>
       </c>
@@ -6755,13 +6755,13 @@
         <v>0</v>
       </c>
       <c r="X63" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y63" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="64" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="64" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A64" s="24" t="s">
         <v>243</v>
       </c>
@@ -6823,13 +6823,13 @@
         <v>0</v>
       </c>
       <c r="X64" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y64" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="65" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="65" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A65" s="24" t="s">
         <v>247</v>
       </c>
@@ -6891,13 +6891,13 @@
         <v>0</v>
       </c>
       <c r="X65" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y65" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="66" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="66" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A66" s="24" t="s">
         <v>251</v>
       </c>
@@ -6959,13 +6959,13 @@
         <v>0</v>
       </c>
       <c r="X66" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y66" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="67" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="67" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A67" s="24" t="s">
         <v>255</v>
       </c>
@@ -7027,13 +7027,13 @@
         <v>0</v>
       </c>
       <c r="X67" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y67" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="68" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="68" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A68" s="24" t="s">
         <v>259</v>
       </c>
@@ -7095,13 +7095,13 @@
         <v>0</v>
       </c>
       <c r="X68" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y68" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="69" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="69" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A69" s="24" t="s">
         <v>264</v>
       </c>
@@ -7163,13 +7163,13 @@
         <v>0</v>
       </c>
       <c r="X69" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y69" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="70" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="70" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A70" s="24" t="s">
         <v>268</v>
       </c>
@@ -7231,13 +7231,13 @@
         <v>0</v>
       </c>
       <c r="X70" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y70" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="71" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="71" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A71" s="24" t="s">
         <v>272</v>
       </c>
@@ -7299,13 +7299,13 @@
         <v>0</v>
       </c>
       <c r="X71" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y71" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="72" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="72" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A72" s="24" t="s">
         <v>276</v>
       </c>
@@ -7367,13 +7367,13 @@
         <v>0</v>
       </c>
       <c r="X72" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y72" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="73" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="73" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A73" s="24" t="s">
         <v>280</v>
       </c>
@@ -7435,13 +7435,13 @@
         <v>0</v>
       </c>
       <c r="X73" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y73" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="74" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="74" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A74" s="24" t="s">
         <v>284</v>
       </c>
@@ -7503,13 +7503,13 @@
         <v>0</v>
       </c>
       <c r="X74" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y74" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="75" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="75" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A75" s="24" t="s">
         <v>288</v>
       </c>
@@ -7571,13 +7571,13 @@
         <v>0</v>
       </c>
       <c r="X75" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y75" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="76" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="76" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A76" s="24" t="s">
         <v>292</v>
       </c>
@@ -7639,13 +7639,13 @@
         <v>0</v>
       </c>
       <c r="X76" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y76" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="77" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="77" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A77" s="24" t="s">
         <v>296</v>
       </c>
@@ -7707,13 +7707,13 @@
         <v>0</v>
       </c>
       <c r="X77" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y77" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="78" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="78" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A78" s="24" t="s">
         <v>300</v>
       </c>
@@ -7775,13 +7775,13 @@
         <v>0</v>
       </c>
       <c r="X78" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y78" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="79" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="79" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A79" s="24" t="s">
         <v>304</v>
       </c>
@@ -7843,13 +7843,13 @@
         <v>0</v>
       </c>
       <c r="X79" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y79" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="80" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="80" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A80" s="24" t="s">
         <v>308</v>
       </c>
@@ -7911,13 +7911,13 @@
         <v>0</v>
       </c>
       <c r="X80" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y80" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="81" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="81" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A81" s="24" t="s">
         <v>312</v>
       </c>
@@ -7979,13 +7979,13 @@
         <v>0</v>
       </c>
       <c r="X81" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y81" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="82" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="82" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A82" s="24" t="s">
         <v>316</v>
       </c>
@@ -8047,13 +8047,13 @@
         <v>0</v>
       </c>
       <c r="X82" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y82" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="83" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="83" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A83" s="24" t="s">
         <v>320</v>
       </c>
@@ -8115,13 +8115,13 @@
         <v>0</v>
       </c>
       <c r="X83" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y83" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="84" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="84" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A84" s="24" t="s">
         <v>324</v>
       </c>
@@ -8183,13 +8183,13 @@
         <v>0</v>
       </c>
       <c r="X84" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y84" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="85" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="85" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A85" s="24" t="s">
         <v>328</v>
       </c>
@@ -8251,13 +8251,13 @@
         <v>0</v>
       </c>
       <c r="X85" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y85" s="27">
         <v>0.6</v>
       </c>
     </row>
-    <row r="86" s="19" customFormat="1" ht="18.75" spans="1:25">
+    <row r="86" s="19" customFormat="1" ht="20.4" spans="1:25">
       <c r="A86" s="24" t="s">
         <v>332</v>
       </c>
@@ -8319,7 +8319,7 @@
         <v>0</v>
       </c>
       <c r="X86" s="19">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y86" s="27">
         <v>0.6</v>
@@ -8339,36 +8339,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="X11" sqref="X11:X20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="3" max="3" width="41.3833333333333" customWidth="1"/>
-    <col min="4" max="4" width="17.6166666666667" customWidth="1"/>
-    <col min="6" max="6" width="18.3083333333333" customWidth="1"/>
-    <col min="7" max="7" width="15.6916666666667" customWidth="1"/>
-    <col min="8" max="8" width="14.6166666666667" customWidth="1"/>
-    <col min="9" max="9" width="17.4583333333333" customWidth="1"/>
-    <col min="10" max="10" width="14.925" customWidth="1"/>
-    <col min="11" max="11" width="13.85" customWidth="1"/>
-    <col min="12" max="12" width="15.15" customWidth="1"/>
-    <col min="13" max="13" width="33.4583333333333" customWidth="1"/>
-    <col min="14" max="14" width="21.15" customWidth="1"/>
+    <col min="3" max="3" width="41.3846153846154" customWidth="1"/>
+    <col min="4" max="4" width="17.6153846153846" customWidth="1"/>
+    <col min="6" max="6" width="18.3076923076923" customWidth="1"/>
+    <col min="7" max="7" width="15.6923076923077" customWidth="1"/>
+    <col min="8" max="8" width="14.6153846153846" customWidth="1"/>
+    <col min="9" max="9" width="17.4615384615385" customWidth="1"/>
+    <col min="10" max="10" width="14.9230769230769" customWidth="1"/>
+    <col min="11" max="11" width="13.8461538461538" customWidth="1"/>
+    <col min="12" max="12" width="15.1538461538462" customWidth="1"/>
+    <col min="13" max="13" width="33.4615384615385" customWidth="1"/>
+    <col min="14" max="14" width="21.1538461538462" customWidth="1"/>
     <col min="15" max="15" width="26" customWidth="1"/>
-    <col min="16" max="16" width="16.4583333333333" customWidth="1"/>
-    <col min="18" max="18" width="21.5416666666667" customWidth="1"/>
-    <col min="19" max="19" width="15.15" customWidth="1"/>
-    <col min="20" max="20" width="21.5416666666667" customWidth="1"/>
-    <col min="23" max="23" width="15.15" customWidth="1"/>
-    <col min="24" max="24" width="27.3083333333333" customWidth="1"/>
-    <col min="25" max="25" width="16.6916666666667" customWidth="1"/>
+    <col min="16" max="16" width="16.4615384615385" customWidth="1"/>
+    <col min="18" max="18" width="21.5384615384615" customWidth="1"/>
+    <col min="19" max="19" width="15.1538461538462" customWidth="1"/>
+    <col min="20" max="20" width="21.5384615384615" customWidth="1"/>
+    <col min="23" max="23" width="15.1538461538462" customWidth="1"/>
+    <col min="24" max="24" width="27.3076923076923" customWidth="1"/>
+    <col min="25" max="25" width="16.6923076923077" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:26">
@@ -8851,7 +8851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" spans="1:26">
+    <row r="7" s="3" customFormat="1" ht="17" spans="1:26">
       <c r="A7" s="10" t="s">
         <v>34</v>
       </c>
@@ -8931,7 +8931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" s="3" customFormat="1" spans="1:26">
+    <row r="8" s="3" customFormat="1" ht="17" spans="1:26">
       <c r="A8" s="10" t="s">
         <v>35</v>
       </c>
@@ -9011,7 +9011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" s="3" customFormat="1" spans="1:26">
+    <row r="9" s="3" customFormat="1" ht="17" spans="1:26">
       <c r="A9" s="10" t="s">
         <v>36</v>
       </c>
@@ -9214,7 +9214,7 @@
         <v>0</v>
       </c>
       <c r="X11" s="5">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y11" s="5" t="s">
         <v>67</v>
@@ -9265,7 +9265,7 @@
         <v>0</v>
       </c>
       <c r="X12" s="5">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y12" s="5" t="s">
         <v>67</v>
@@ -9316,7 +9316,7 @@
         <v>0</v>
       </c>
       <c r="X13" s="5">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y13" s="5" t="s">
         <v>67</v>
@@ -9367,7 +9367,7 @@
         <v>0</v>
       </c>
       <c r="X14" s="5">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y14" s="5" t="s">
         <v>67</v>
@@ -9418,7 +9418,7 @@
         <v>0</v>
       </c>
       <c r="X15" s="5">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y15" s="5" t="s">
         <v>67</v>
@@ -9469,7 +9469,7 @@
         <v>0</v>
       </c>
       <c r="X16" s="5">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y16" s="5" t="s">
         <v>67</v>
@@ -9520,7 +9520,7 @@
         <v>0</v>
       </c>
       <c r="X17" s="5">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y17" s="5" t="s">
         <v>67</v>
@@ -9571,7 +9571,7 @@
         <v>0</v>
       </c>
       <c r="X18" s="5">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y18" s="5" t="s">
         <v>67</v>
@@ -9622,7 +9622,7 @@
         <v>0</v>
       </c>
       <c r="X19" s="5">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y19" s="5" t="s">
         <v>67</v>
@@ -9673,7 +9673,7 @@
         <v>0</v>
       </c>
       <c r="X20" s="5">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y20" s="5" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
modify consume value type as integer from string.
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Skill.xlsx
+++ b/_Out/NFDataCfg/Excel/Skill.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63">
   <si>
     <t>Id</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>SendBuffList</t>
+  </si>
+  <si>
+    <t>ScriptObject</t>
   </si>
   <si>
     <t>CoolDownTime</t>
@@ -152,6 +155,9 @@
     <t>使用后对方获得的BUFF</t>
   </si>
   <si>
+    <t>script file</t>
+  </si>
+  <si>
     <t>使用冷却CD</t>
   </si>
   <si>
@@ -215,10 +221,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -252,8 +258,46 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -267,14 +311,52 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -291,39 +373,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -331,44 +383,6 @@
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -380,7 +394,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -389,15 +403,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -442,13 +448,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,19 +526,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -484,7 +556,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,25 +586,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -526,91 +610,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -710,6 +716,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -749,15 +764,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -769,6 +775,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -796,164 +813,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1399,10 +1405,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:U20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I11" sqref="I11:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1419,13 +1425,13 @@
     <col min="12" max="12" width="14.9230769230769" customWidth="1"/>
     <col min="13" max="13" width="21.1538461538462" customWidth="1"/>
     <col min="14" max="14" width="26" customWidth="1"/>
-    <col min="15" max="15" width="16.4615384615385" customWidth="1"/>
-    <col min="16" max="16" width="21.5384615384615" customWidth="1"/>
-    <col min="19" max="19" width="27.3076923076923" customWidth="1"/>
-    <col min="20" max="20" width="16.6923076923077" customWidth="1"/>
+    <col min="15" max="16" width="16.4615384615385" customWidth="1"/>
+    <col min="17" max="17" width="21.5384615384615" customWidth="1"/>
+    <col min="20" max="20" width="27.3076923076923" customWidth="1"/>
+    <col min="21" max="21" width="16.6923076923077" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:20">
+    <row r="1" s="1" customFormat="1" spans="1:21">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1486,72 +1492,78 @@
       <c r="T1" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="U1" s="7" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" s="2" customFormat="1" spans="1:20">
+    <row r="2" s="2" customFormat="1" spans="1:21">
       <c r="A2" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>22</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="9" t="s">
-        <v>21</v>
-      </c>
       <c r="M2" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O2" s="9" t="s">
         <v>23</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="S2" s="9" t="s">
         <v>23</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="1" spans="1:20">
+    <row r="3" s="2" customFormat="1" spans="1:21">
       <c r="A3" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" s="9">
         <v>0</v>
@@ -1610,10 +1622,13 @@
       <c r="T3" s="9">
         <v>0</v>
       </c>
+      <c r="U3" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" s="2" customFormat="1" spans="1:20">
+    <row r="4" s="2" customFormat="1" spans="1:21">
       <c r="A4" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B4" s="9">
         <v>0</v>
@@ -1672,10 +1687,13 @@
       <c r="T4" s="9">
         <v>0</v>
       </c>
+      <c r="U4" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" s="2" customFormat="1" spans="1:20">
+    <row r="5" s="2" customFormat="1" spans="1:21">
       <c r="A5" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5" s="9">
         <v>0</v>
@@ -1734,10 +1752,13 @@
       <c r="T5" s="9">
         <v>0</v>
       </c>
+      <c r="U5" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" s="2" customFormat="1" spans="1:20">
+    <row r="6" s="2" customFormat="1" spans="1:21">
       <c r="A6" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="9">
         <v>0</v>
@@ -1796,10 +1817,13 @@
       <c r="T6" s="9">
         <v>0</v>
       </c>
+      <c r="U6" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" s="3" customFormat="1" ht="17" spans="1:20">
+    <row r="7" s="3" customFormat="1" ht="17" spans="1:21">
       <c r="A7" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" s="11">
         <v>0</v>
@@ -1858,10 +1882,13 @@
       <c r="T7" s="11">
         <v>0</v>
       </c>
+      <c r="U7" s="11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" s="3" customFormat="1" ht="17" spans="1:20">
+    <row r="8" s="3" customFormat="1" ht="17" spans="1:21">
       <c r="A8" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8" s="11">
         <v>0</v>
@@ -1920,10 +1947,13 @@
       <c r="T8" s="11">
         <v>0</v>
       </c>
+      <c r="U8" s="11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" s="3" customFormat="1" ht="17" spans="1:20">
+    <row r="9" s="3" customFormat="1" ht="17" spans="1:21">
       <c r="A9" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B9" s="11">
         <v>0</v>
@@ -1982,72 +2012,78 @@
       <c r="T9" s="11">
         <v>0</v>
       </c>
+      <c r="U9" s="11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" s="4" customFormat="1" ht="17" customHeight="1" spans="1:20">
+    <row r="10" s="4" customFormat="1" ht="17" customHeight="1" spans="1:21">
       <c r="A10" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M10" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N10" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O10" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P10" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q10" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="R10" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="S10" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="T10" s="11" t="s">
         <v>47</v>
       </c>
+      <c r="T10" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="U10" s="11" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="11" s="5" customFormat="1" spans="1:20">
+    <row r="11" s="5" customFormat="1" spans="1:21">
       <c r="A11" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B11" s="5">
         <v>0</v>
@@ -2059,356 +2095,386 @@
         <v>0</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F11" s="15"/>
+      <c r="I11" s="5">
+        <v>0</v>
+      </c>
       <c r="J11" s="5">
         <v>0</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L11" s="16">
         <v>130</v>
       </c>
-      <c r="O11" s="5">
+      <c r="P11" s="5">
         <v>1</v>
       </c>
-      <c r="S11" s="5">
+      <c r="T11" s="5">
         <v>3</v>
       </c>
-      <c r="T11" s="5" t="s">
+      <c r="U11" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" s="5" customFormat="1" spans="1:21">
+      <c r="A12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="14" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" s="5" customFormat="1" spans="1:20">
-      <c r="A12" s="5" t="s">
+      <c r="F12" s="15"/>
+      <c r="I12" s="5">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5">
+        <v>0</v>
+      </c>
+      <c r="K12" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="B12" s="5">
-        <v>0</v>
-      </c>
-      <c r="C12" s="5">
-        <v>0</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="15"/>
-      <c r="J12" s="5">
-        <v>0</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>50</v>
       </c>
       <c r="L12" s="16">
         <v>130</v>
       </c>
-      <c r="O12" s="5">
+      <c r="P12" s="5">
         <v>1</v>
       </c>
-      <c r="S12" s="5">
+      <c r="T12" s="5">
         <v>3</v>
       </c>
-      <c r="T12" s="5" t="s">
+      <c r="U12" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" s="5" customFormat="1" spans="1:21">
+      <c r="A13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="13" s="5" customFormat="1" spans="1:20">
-      <c r="A13" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="5">
-        <v>0</v>
-      </c>
-      <c r="C13" s="5">
-        <v>0</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>49</v>
-      </c>
       <c r="F13" s="15"/>
+      <c r="I13" s="5">
+        <v>0</v>
+      </c>
       <c r="J13" s="5">
         <v>0</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L13" s="16">
         <v>130</v>
       </c>
-      <c r="O13" s="5">
+      <c r="P13" s="5">
         <v>1</v>
       </c>
-      <c r="S13" s="5">
+      <c r="T13" s="5">
         <v>3</v>
       </c>
-      <c r="T13" s="5" t="s">
+      <c r="U13" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" s="5" customFormat="1" spans="1:21">
+      <c r="A14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="5">
+        <v>0</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0</v>
+      </c>
+      <c r="E14" s="14" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" s="5" customFormat="1" spans="1:20">
-      <c r="A14" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="5">
-        <v>0</v>
-      </c>
-      <c r="C14" s="5">
-        <v>0</v>
-      </c>
-      <c r="D14" s="5">
-        <v>0</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>49</v>
-      </c>
       <c r="F14" s="15"/>
+      <c r="I14" s="5">
+        <v>0</v>
+      </c>
       <c r="J14" s="5">
         <v>0</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L14" s="16">
         <v>130</v>
       </c>
-      <c r="O14" s="5">
+      <c r="P14" s="5">
         <v>1</v>
       </c>
-      <c r="S14" s="5">
+      <c r="T14" s="5">
         <v>3</v>
       </c>
-      <c r="T14" s="5" t="s">
+      <c r="U14" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" s="5" customFormat="1" spans="1:21">
+      <c r="A15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0</v>
+      </c>
+      <c r="E15" s="14" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="15" s="5" customFormat="1" spans="1:20">
-      <c r="A15" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="5">
-        <v>0</v>
-      </c>
-      <c r="C15" s="5">
-        <v>0</v>
-      </c>
-      <c r="D15" s="5">
-        <v>0</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>49</v>
-      </c>
       <c r="F15" s="15"/>
+      <c r="I15" s="5">
+        <v>0</v>
+      </c>
       <c r="J15" s="5">
         <v>0</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L15" s="16">
         <v>130</v>
       </c>
-      <c r="O15" s="5">
+      <c r="P15" s="5">
         <v>1</v>
       </c>
-      <c r="S15" s="5">
+      <c r="T15" s="5">
         <v>3</v>
       </c>
-      <c r="T15" s="5" t="s">
+      <c r="U15" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" s="5" customFormat="1" spans="1:21">
+      <c r="A16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0</v>
+      </c>
+      <c r="E16" s="14" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="16" s="5" customFormat="1" spans="1:20">
-      <c r="A16" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="5">
-        <v>0</v>
-      </c>
-      <c r="C16" s="5">
-        <v>0</v>
-      </c>
-      <c r="D16" s="5">
-        <v>0</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>49</v>
-      </c>
       <c r="F16" s="15"/>
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
       <c r="J16" s="5">
         <v>0</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L16" s="16">
         <v>130</v>
       </c>
-      <c r="O16" s="5">
+      <c r="P16" s="5">
         <v>1</v>
       </c>
-      <c r="S16" s="5">
+      <c r="T16" s="5">
         <v>3</v>
       </c>
-      <c r="T16" s="5" t="s">
+      <c r="U16" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" s="5" customFormat="1" spans="1:21">
+      <c r="A17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0</v>
+      </c>
+      <c r="E17" s="14" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" s="5" customFormat="1" spans="1:20">
-      <c r="A17" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B17" s="5">
-        <v>0</v>
-      </c>
-      <c r="C17" s="5">
-        <v>0</v>
-      </c>
-      <c r="D17" s="5">
-        <v>0</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>49</v>
-      </c>
       <c r="F17" s="15"/>
+      <c r="I17" s="5">
+        <v>0</v>
+      </c>
       <c r="J17" s="5">
         <v>0</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L17" s="16">
         <v>130</v>
       </c>
-      <c r="O17" s="5">
+      <c r="P17" s="5">
         <v>1</v>
       </c>
-      <c r="S17" s="5">
+      <c r="T17" s="5">
         <v>3</v>
       </c>
-      <c r="T17" s="5" t="s">
+      <c r="U17" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" s="5" customFormat="1" spans="1:21">
+      <c r="A18" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" s="5" customFormat="1" spans="1:20">
-      <c r="A18" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" s="5">
-        <v>0</v>
-      </c>
-      <c r="C18" s="5">
-        <v>0</v>
-      </c>
-      <c r="D18" s="5">
-        <v>0</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>49</v>
-      </c>
       <c r="F18" s="15"/>
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
       <c r="J18" s="5">
         <v>0</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L18" s="16">
         <v>130</v>
       </c>
-      <c r="O18" s="5">
+      <c r="P18" s="5">
         <v>1</v>
       </c>
-      <c r="S18" s="5">
+      <c r="T18" s="5">
         <v>3</v>
       </c>
-      <c r="T18" s="5" t="s">
+      <c r="U18" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" s="5" customFormat="1" spans="1:21">
+      <c r="A19" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
+      <c r="E19" s="14" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" s="5" customFormat="1" spans="1:20">
-      <c r="A19" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="5">
-        <v>0</v>
-      </c>
-      <c r="C19" s="5">
-        <v>0</v>
-      </c>
-      <c r="D19" s="5">
-        <v>0</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>49</v>
-      </c>
       <c r="F19" s="15"/>
+      <c r="I19" s="5">
+        <v>0</v>
+      </c>
       <c r="J19" s="5">
         <v>0</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L19" s="16">
         <v>130</v>
       </c>
-      <c r="O19" s="5">
+      <c r="P19" s="5">
         <v>1</v>
       </c>
-      <c r="S19" s="5">
+      <c r="T19" s="5">
         <v>3</v>
       </c>
-      <c r="T19" s="5" t="s">
+      <c r="U19" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" s="5" customFormat="1" spans="1:21">
+      <c r="A20" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0</v>
+      </c>
+      <c r="D20" s="5">
+        <v>0</v>
+      </c>
+      <c r="E20" s="14" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" s="5" customFormat="1" spans="1:20">
-      <c r="A20" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="5">
-        <v>0</v>
-      </c>
-      <c r="C20" s="5">
-        <v>0</v>
-      </c>
-      <c r="D20" s="5">
-        <v>0</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>49</v>
-      </c>
       <c r="F20" s="15"/>
+      <c r="I20" s="5">
+        <v>0</v>
+      </c>
       <c r="J20" s="5">
         <v>0</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L20" s="16">
         <v>130</v>
       </c>
-      <c r="O20" s="5">
+      <c r="P20" s="5">
         <v>1</v>
       </c>
-      <c r="S20" s="5">
+      <c r="T20" s="5">
         <v>3</v>
       </c>
-      <c r="T20" s="5" t="s">
-        <v>51</v>
+      <c r="U20" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B9 C7:C9 D7:D9 S7:T9 E7:L9 M7:O9 P7:R9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B9 C7:C9 D7:D9 O7:O9 P7:P9 M7:N9 E7:L9 T7:U9 Q7:S9">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>